<commit_message>
cam binding to camkii no longer bimolecular rxn
</commit_message>
<xml_diff>
--- a/rxns_table.xlsx
+++ b/rxns_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD_2023\CaMKII_hexa_bgnl_to_mcell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA4DAF3F-4E8A-48B9-AC60-42DB75336887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A912B24B-F54D-4E58-A153-33ADB87BA176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4B4FB280-5B08-406D-B059-D87F72317E26}"/>
   </bookViews>
@@ -593,12 +593,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -977,12 +984,12 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="53.36328125" customWidth="1"/>
+    <col min="1" max="1" width="41.453125" style="6" customWidth="1"/>
     <col min="2" max="2" width="25.08984375" customWidth="1"/>
     <col min="3" max="3" width="11.08984375" customWidth="1"/>
     <col min="4" max="4" width="11.90625" customWidth="1"/>
@@ -992,7 +999,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1014,83 +1021,95 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>1000000</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7"/>
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>1000000</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7"/>
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>1000000</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7"/>
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>1000000</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
+      <c r="C6" s="2">
+        <v>20000</v>
+      </c>
       <c r="E6" t="s">
         <v>15</v>
       </c>
+      <c r="F6" s="2">
+        <v>10000000</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:7" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="C7" s="4">
+        <v>4200000</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1120,27 +1139,27 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cam binding to camkii IS bimolecular, previous commit was wrong
</commit_message>
<xml_diff>
--- a/rxns_table.xlsx
+++ b/rxns_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD_2023\CaMKII_hexa_bgnl_to_mcell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A912B24B-F54D-4E58-A153-33ADB87BA176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AC92C6-FD08-4472-9E0F-9A95B65441CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4B4FB280-5B08-406D-B059-D87F72317E26}"/>
   </bookViews>
@@ -246,7 +246,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -429,6 +429,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -593,19 +599,20 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="16" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" xfId="16" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -984,12 +991,12 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.453125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="41.453125" style="4" customWidth="1"/>
     <col min="2" max="2" width="25.08984375" customWidth="1"/>
     <col min="3" max="3" width="11.08984375" customWidth="1"/>
     <col min="4" max="4" width="11.90625" customWidth="1"/>
@@ -999,7 +1006,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1021,145 +1028,155 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>1000000</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="5"/>
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>1000000</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="5"/>
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>1000000</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="7"/>
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5"/>
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>1000000</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>20000</v>
       </c>
       <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>10000000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:7" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>4200000</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="6" t="s">
         <v>27</v>
       </c>
       <c r="E8" t="s">
         <v>19</v>
       </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="6" t="s">
         <v>27</v>
       </c>
       <c r="E9" t="s">
         <v>20</v>
       </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="C10" s="3">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B11" t="s">
         <v>24</v>
       </c>
+      <c r="C11">
+        <v>0.02</v>
+      </c>
     </row>
-    <row r="12" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
camkii t306 P conditions changed according to literature; and xlsx references added
</commit_message>
<xml_diff>
--- a/rxns_table.xlsx
+++ b/rxns_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD_2023\CaMKII_hexa_bgnl_to_mcell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AC92C6-FD08-4472-9E0F-9A95B65441CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF044C3-81FD-4502-9D9E-5BD144684724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4B4FB280-5B08-406D-B059-D87F72317E26}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4B4FB280-5B08-406D-B059-D87F72317E26}"/>
   </bookViews>
   <sheets>
     <sheet name="rxns_table" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>Description</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Stefan et al., 2012; Pharris et al., 2020</t>
+  </si>
+  <si>
+    <t>Pharris et al., 2020</t>
   </si>
 </sst>
 </file>
@@ -599,7 +605,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -613,6 +619,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="16" quotePrefix="1"/>
     <xf numFmtId="0" fontId="15" fillId="33" borderId="0" xfId="16" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -991,21 +1000,21 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.453125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="25.08984375" customWidth="1"/>
-    <col min="3" max="3" width="11.08984375" customWidth="1"/>
-    <col min="4" max="4" width="11.90625" customWidth="1"/>
-    <col min="5" max="5" width="26.81640625" customWidth="1"/>
-    <col min="6" max="6" width="13.36328125" customWidth="1"/>
-    <col min="7" max="7" width="15.1796875" customWidth="1"/>
+    <col min="1" max="1" width="41.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1028,7 +1037,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1041,8 +1050,11 @@
       <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="F2" s="2">
+        <v>1.9279999999999999</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="2" t="s">
         <v>7</v>
@@ -1053,8 +1065,11 @@
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="F3" s="2">
+        <v>1.9370000000000001</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -1065,8 +1080,11 @@
       <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="F4" s="2">
+        <v>7.476</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="2" t="s">
         <v>11</v>
@@ -1077,8 +1095,11 @@
       <c r="E5" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="F5" s="2">
+        <v>25.783000000000001</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -1088,14 +1109,20 @@
       <c r="C6" s="1">
         <v>20000</v>
       </c>
+      <c r="D6" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="E6" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="1">
         <v>10000000</v>
       </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
@@ -1115,7 +1142,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -1134,7 +1161,7 @@
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>27</v>
       </c>
@@ -1150,7 +1177,7 @@
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
@@ -1161,7 +1188,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
@@ -1172,15 +1199,19 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>26</v>
+      </c>
+      <c r="C12" s="3">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reactions in excel doc updated
</commit_message>
<xml_diff>
--- a/rxns_table.xlsx
+++ b/rxns_table.xlsx
@@ -1,26 +1,91 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD_2023\CaMKII_hexa_bgnl_to_mcell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF044C3-81FD-4502-9D9E-5BD144684724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E7EA75-C412-41F4-93C7-373E5DA996DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4B4FB280-5B08-406D-B059-D87F72317E26}"/>
+    <workbookView xWindow="-19310" yWindow="1260" windowWidth="19420" windowHeight="10420" xr2:uid="{4B4FB280-5B08-406D-B059-D87F72317E26}"/>
   </bookViews>
   <sheets>
     <sheet name="rxns_table" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={B6F8C469-337C-40BE-B2DC-A13B6B68197A}</author>
+    <author>Susana Roman</author>
+    <author>tc={6C2818CD-9DCB-407F-A713-A0F009955982}</author>
+  </authors>
+  <commentList>
+    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{B6F8C469-337C-40BE-B2DC-A13B6B68197A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not modelled currently; we specify different off rates depending on whether camkii is P or not.</t>
+      </text>
+    </comment>
+    <comment ref="L22" authorId="1" shapeId="0" xr:uid="{D783E934-AE8E-45F6-BF32-CFA5F3DEAB20}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Susana Roman:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+with cam_ca4 bound to camkii</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N25" authorId="2" shapeId="0" xr:uid="{6C2818CD-9DCB-407F-A713-A0F009955982}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    In this paper there is also k_mPP1 and k_onPP1 which should be checked to see how they are used</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="51">
   <si>
     <t>Description</t>
   </si>
@@ -28,39 +93,9 @@
     <t>Parameter</t>
   </si>
   <si>
-    <t>Value</t>
-  </si>
-  <si>
     <t>Reference</t>
   </si>
   <si>
-    <t>Calcium binds to CaM progresively</t>
-  </si>
-  <si>
-    <t>kon_1_CaCaM</t>
-  </si>
-  <si>
-    <t>koff_1_CaCaM</t>
-  </si>
-  <si>
-    <t>kon_2_CaCaM</t>
-  </si>
-  <si>
-    <t>koff_2_CaCaM</t>
-  </si>
-  <si>
-    <t>kon_3_CaCaM</t>
-  </si>
-  <si>
-    <t>koff_3_CaCaM</t>
-  </si>
-  <si>
-    <t>kon_4_CaCaM</t>
-  </si>
-  <si>
-    <t>koff_4_CaCaM</t>
-  </si>
-  <si>
     <t>CaMKII subunits active/inactive flicker</t>
   </si>
   <si>
@@ -70,15 +105,9 @@
     <t>koff_CaMKII_inact</t>
   </si>
   <si>
-    <t>CaM binds to CaMKII. Saturated CaM_Ca4 binds to CaMKII(T306~0, active~1)</t>
-  </si>
-  <si>
     <t>kon_CaM_Ca4_CaMKII</t>
   </si>
   <si>
-    <t>CaM unbinds from CaMKII. Wether CaMKII(T286~P) or CaMKII(T286~0)</t>
-  </si>
-  <si>
     <t>koff_CaM_Ca4_CaMKII286_P</t>
   </si>
   <si>
@@ -103,20 +132,119 @@
     <t>Kcat</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Stefan et al., 2012; Pharris et al., 2020</t>
   </si>
   <si>
     <t>Pharris et al., 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter </t>
+  </si>
+  <si>
+    <t>Value (1/Ms)</t>
+  </si>
+  <si>
+    <t>dissertation</t>
+  </si>
+  <si>
+    <t>Ordyan et al., 2020</t>
+  </si>
+  <si>
+    <t>Faas et al., 2011</t>
+  </si>
+  <si>
+    <t>Pepke et al., 2010</t>
+  </si>
+  <si>
+    <t>given as range</t>
+  </si>
+  <si>
+    <t>Li et al., 2019</t>
+  </si>
+  <si>
+    <t>Bartol et al., 2024</t>
+  </si>
+  <si>
+    <t>Value (1/s)</t>
+  </si>
+  <si>
+    <t>kon_3_CaCaM -C</t>
+  </si>
+  <si>
+    <t>kon_4_CaCaM -C</t>
+  </si>
+  <si>
+    <t>kon_1_CaCaM -N</t>
+  </si>
+  <si>
+    <t>kon_2_CaCaM -N</t>
+  </si>
+  <si>
+    <t>koff_1_CaCaM -N</t>
+  </si>
+  <si>
+    <t>koff_2_CaCaM -N</t>
+  </si>
+  <si>
+    <t>koff_3_CaCaM -C</t>
+  </si>
+  <si>
+    <t>koff_4_CaCaM -C</t>
+  </si>
+  <si>
+    <t>Value (M)</t>
+  </si>
+  <si>
+    <t>koff_CaM_Ca4_CaMKII</t>
+  </si>
+  <si>
+    <t>-----</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>kon_CaM_Ca4_CaMKII286_0</t>
+  </si>
+  <si>
+    <t>kon_CaM_Ca4_CaMKII286_P</t>
+  </si>
+  <si>
+    <t>tbc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calcium unbinds from CaM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calcium binds to CaM </t>
+  </si>
+  <si>
+    <t>CaM_Ca4 unbinds from CaMKII. Wether CaMKII(T286~P) or CaMKII(T286~0)</t>
+  </si>
+  <si>
+    <t>CaM binds to CaMKII. Only saturated CaM_Ca4 binds to CaMKII(T306~0, active~1)</t>
+  </si>
+  <si>
+    <t>CaMKII binding to NMDARs</t>
+  </si>
+  <si>
+    <t>Coultrap at al., 2012</t>
+  </si>
+  <si>
+    <t>0.03-0.71</t>
+  </si>
+  <si>
+    <t>Lucic et al., 2008</t>
+  </si>
+  <si>
+    <t>CaMKII</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,8 +379,67 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -440,7 +627,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE781"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -605,7 +822,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -613,15 +830,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="22" fillId="4" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="11" fontId="21" fillId="4" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="16" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" xfId="16" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="21" fillId="36" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="22" fillId="36" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="36" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="21" fillId="36" borderId="0" xfId="6" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="18" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="21" fillId="36" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="22" fillId="36" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="23" fillId="36" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="21" fillId="37" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="22" fillId="37" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="21" fillId="37" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="13"/>
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="18" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="39" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="18" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -669,6 +927,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFE781"/>
+      <color rgb="FFFFE265"/>
+      <color rgb="FFFFFFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -678,6 +943,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Susana Roman" id="{48458BD6-4CAC-498F-B01C-BB6F89FD41FA}" userId="628ed1ff9e8d383f" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -995,223 +1266,2316 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B18" dT="2024-08-07T13:14:12.40" personId="{48458BD6-4CAC-498F-B01C-BB6F89FD41FA}" id="{B6F8C469-337C-40BE-B2DC-A13B6B68197A}">
+    <text>Not modelled currently; we specify different off rates depending on whether camkii is P or not.</text>
+  </threadedComment>
+  <threadedComment ref="N25" dT="2024-08-08T08:46:52.90" personId="{48458BD6-4CAC-498F-B01C-BB6F89FD41FA}" id="{6C2818CD-9DCB-407F-A713-A0F009955982}">
+    <text>In this paper there is also k_mPP1 and k_onPP1 which should be checked to see how they are used</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B603CBE9-61C1-43B8-82FF-7D32E551985B}">
-  <dimension ref="A1:G12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B603CBE9-61C1-43B8-82FF-7D32E551985B}">
+  <dimension ref="A1:CU27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="44.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="9" width="11.7109375" customWidth="1"/>
+    <col min="10" max="11" width="11.7109375" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+    <col min="13" max="15" width="14.5703125" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" customWidth="1"/>
+    <col min="19" max="19" width="11" customWidth="1"/>
+    <col min="20" max="29" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:99" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:99" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="17">
+        <v>1000000</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="31">
+        <v>25000000</v>
+      </c>
+      <c r="F2" s="31">
+        <v>260000000</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="17">
+        <v>770000000</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="26">
+        <v>32200000000</v>
+      </c>
+      <c r="K2" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="35">
+        <v>100000000</v>
+      </c>
+      <c r="M2" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="26">
+        <v>100000000</v>
+      </c>
+      <c r="O2" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+      <c r="Z2"/>
+      <c r="AA2"/>
+      <c r="AB2"/>
+      <c r="AC2"/>
+      <c r="AD2"/>
+      <c r="AE2"/>
+      <c r="AF2"/>
+      <c r="AG2"/>
+      <c r="AH2"/>
+      <c r="AI2"/>
+      <c r="AJ2"/>
+      <c r="AK2"/>
+      <c r="AL2"/>
+      <c r="AM2"/>
+      <c r="AN2"/>
+      <c r="AO2"/>
+      <c r="AP2"/>
+      <c r="AQ2"/>
+      <c r="AR2"/>
+      <c r="AS2"/>
+      <c r="AT2"/>
+      <c r="AU2"/>
+      <c r="AV2"/>
+      <c r="AW2"/>
+      <c r="AX2"/>
+      <c r="AY2"/>
+      <c r="AZ2"/>
+      <c r="BA2"/>
+      <c r="BB2"/>
+      <c r="BC2"/>
+      <c r="BD2"/>
+      <c r="BE2"/>
+      <c r="BF2"/>
+      <c r="BG2"/>
+      <c r="BH2"/>
+      <c r="BI2"/>
+      <c r="BJ2"/>
+      <c r="BK2"/>
+      <c r="BL2"/>
+      <c r="BM2"/>
+      <c r="BN2"/>
+      <c r="BO2"/>
+      <c r="BP2"/>
+      <c r="BQ2"/>
+      <c r="BR2"/>
+      <c r="BS2"/>
+      <c r="BT2"/>
+      <c r="BU2"/>
+      <c r="BV2"/>
+      <c r="BW2"/>
+      <c r="BX2"/>
+      <c r="BY2"/>
+      <c r="BZ2"/>
+      <c r="CA2"/>
+      <c r="CB2"/>
+      <c r="CC2"/>
+      <c r="CD2"/>
+      <c r="CE2"/>
+      <c r="CF2"/>
+      <c r="CG2"/>
+      <c r="CH2"/>
+      <c r="CI2"/>
+      <c r="CJ2"/>
+      <c r="CK2"/>
+      <c r="CL2"/>
+      <c r="CM2"/>
+      <c r="CN2"/>
+      <c r="CO2"/>
+      <c r="CP2"/>
+      <c r="CQ2"/>
+      <c r="CR2"/>
+      <c r="CS2"/>
+      <c r="CT2"/>
+      <c r="CU2"/>
+    </row>
+    <row r="3" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="17">
+        <v>1000000</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="31">
+        <v>50000000</v>
+      </c>
+      <c r="F3" s="31">
+        <v>300000000</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="17">
+        <v>32000000000</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="26">
+        <v>32200000000</v>
+      </c>
+      <c r="K3" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="35">
+        <v>150000000</v>
+      </c>
+      <c r="M3" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="26">
+        <v>150000000</v>
+      </c>
+      <c r="O3" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+      <c r="Y3"/>
+      <c r="Z3"/>
+      <c r="AA3"/>
+      <c r="AB3"/>
+      <c r="AC3"/>
+      <c r="AD3"/>
+      <c r="AE3"/>
+      <c r="AF3"/>
+      <c r="AG3"/>
+      <c r="AH3"/>
+      <c r="AI3"/>
+      <c r="AJ3"/>
+      <c r="AK3"/>
+      <c r="AL3"/>
+      <c r="AM3"/>
+      <c r="AN3"/>
+      <c r="AO3"/>
+      <c r="AP3"/>
+      <c r="AQ3"/>
+      <c r="AR3"/>
+      <c r="AS3"/>
+      <c r="AT3"/>
+      <c r="AU3"/>
+      <c r="AV3"/>
+      <c r="AW3"/>
+      <c r="AX3"/>
+      <c r="AY3"/>
+      <c r="AZ3"/>
+      <c r="BA3"/>
+      <c r="BB3"/>
+      <c r="BC3"/>
+      <c r="BD3"/>
+      <c r="BE3"/>
+      <c r="BF3"/>
+      <c r="BG3"/>
+      <c r="BH3"/>
+      <c r="BI3"/>
+      <c r="BJ3"/>
+      <c r="BK3"/>
+      <c r="BL3"/>
+      <c r="BM3"/>
+      <c r="BN3"/>
+      <c r="BO3"/>
+      <c r="BP3"/>
+      <c r="BQ3"/>
+      <c r="BR3"/>
+      <c r="BS3"/>
+      <c r="BT3"/>
+      <c r="BU3"/>
+      <c r="BV3"/>
+      <c r="BW3"/>
+      <c r="BX3"/>
+      <c r="BY3"/>
+      <c r="BZ3"/>
+      <c r="CA3"/>
+      <c r="CB3"/>
+      <c r="CC3"/>
+      <c r="CD3"/>
+      <c r="CE3"/>
+      <c r="CF3"/>
+      <c r="CG3"/>
+      <c r="CH3"/>
+      <c r="CI3"/>
+      <c r="CJ3"/>
+      <c r="CK3"/>
+      <c r="CL3"/>
+      <c r="CM3"/>
+      <c r="CN3"/>
+      <c r="CO3"/>
+      <c r="CP3"/>
+      <c r="CQ3"/>
+      <c r="CR3"/>
+      <c r="CS3"/>
+      <c r="CT3"/>
+      <c r="CU3"/>
+    </row>
+    <row r="4" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="17">
+        <v>1000000</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="31">
+        <v>1200000</v>
+      </c>
+      <c r="F4" s="31">
+        <v>9600000</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="17">
+        <v>84000000</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="26">
+        <v>322000000</v>
+      </c>
+      <c r="K4" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="35">
+        <v>4000000</v>
+      </c>
+      <c r="M4" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="26">
+        <v>4000000</v>
+      </c>
+      <c r="O4" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4"/>
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4"/>
+      <c r="Y4"/>
+      <c r="Z4"/>
+      <c r="AA4"/>
+      <c r="AB4"/>
+      <c r="AC4"/>
+      <c r="AD4"/>
+      <c r="AE4"/>
+      <c r="AF4"/>
+      <c r="AG4"/>
+      <c r="AH4"/>
+      <c r="AI4"/>
+      <c r="AJ4"/>
+      <c r="AK4"/>
+      <c r="AL4"/>
+      <c r="AM4"/>
+      <c r="AN4"/>
+      <c r="AO4"/>
+      <c r="AP4"/>
+      <c r="AQ4"/>
+      <c r="AR4"/>
+      <c r="AS4"/>
+      <c r="AT4"/>
+      <c r="AU4"/>
+      <c r="AV4"/>
+      <c r="AW4"/>
+      <c r="AX4"/>
+      <c r="AY4"/>
+      <c r="AZ4"/>
+      <c r="BA4"/>
+      <c r="BB4"/>
+      <c r="BC4"/>
+      <c r="BD4"/>
+      <c r="BE4"/>
+      <c r="BF4"/>
+      <c r="BG4"/>
+      <c r="BH4"/>
+      <c r="BI4"/>
+      <c r="BJ4"/>
+      <c r="BK4"/>
+      <c r="BL4"/>
+      <c r="BM4"/>
+      <c r="BN4"/>
+      <c r="BO4"/>
+      <c r="BP4"/>
+      <c r="BQ4"/>
+      <c r="BR4"/>
+      <c r="BS4"/>
+      <c r="BT4"/>
+      <c r="BU4"/>
+      <c r="BV4"/>
+      <c r="BW4"/>
+      <c r="BX4"/>
+      <c r="BY4"/>
+      <c r="BZ4"/>
+      <c r="CA4"/>
+      <c r="CB4"/>
+      <c r="CC4"/>
+      <c r="CD4"/>
+      <c r="CE4"/>
+      <c r="CF4"/>
+      <c r="CG4"/>
+      <c r="CH4"/>
+      <c r="CI4"/>
+      <c r="CJ4"/>
+      <c r="CK4"/>
+      <c r="CL4"/>
+      <c r="CM4"/>
+      <c r="CN4"/>
+      <c r="CO4"/>
+      <c r="CP4"/>
+      <c r="CQ4"/>
+      <c r="CR4"/>
+      <c r="CS4"/>
+      <c r="CT4"/>
+      <c r="CU4"/>
+    </row>
+    <row r="5" spans="1:99" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12"/>
+      <c r="B5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="17">
+        <v>1000000</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="31">
+        <v>5000000</v>
+      </c>
+      <c r="F5" s="31">
+        <v>25000000</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="17">
+        <v>250000000</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="26">
+        <v>322000000</v>
+      </c>
+      <c r="K5" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="35">
+        <v>10000000</v>
+      </c>
+      <c r="M5" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" s="26">
+        <v>10000000</v>
+      </c>
+      <c r="O5" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
+      <c r="X5"/>
+      <c r="Y5"/>
+      <c r="Z5"/>
+      <c r="AA5"/>
+      <c r="AB5"/>
+      <c r="AC5"/>
+      <c r="AD5"/>
+      <c r="AE5"/>
+      <c r="AF5"/>
+      <c r="AG5"/>
+      <c r="AH5"/>
+      <c r="AI5"/>
+      <c r="AJ5"/>
+      <c r="AK5"/>
+      <c r="AL5"/>
+      <c r="AM5"/>
+      <c r="AN5"/>
+      <c r="AO5"/>
+      <c r="AP5"/>
+      <c r="AQ5"/>
+      <c r="AR5"/>
+      <c r="AS5"/>
+      <c r="AT5"/>
+      <c r="AU5"/>
+      <c r="AV5"/>
+      <c r="AW5"/>
+      <c r="AX5"/>
+      <c r="AY5"/>
+      <c r="AZ5"/>
+      <c r="BA5"/>
+      <c r="BB5"/>
+      <c r="BC5"/>
+      <c r="BD5"/>
+      <c r="BE5"/>
+      <c r="BF5"/>
+      <c r="BG5"/>
+      <c r="BH5"/>
+      <c r="BI5"/>
+      <c r="BJ5"/>
+      <c r="BK5"/>
+      <c r="BL5"/>
+      <c r="BM5"/>
+      <c r="BN5"/>
+      <c r="BO5"/>
+      <c r="BP5"/>
+      <c r="BQ5"/>
+      <c r="BR5"/>
+      <c r="BS5"/>
+      <c r="BT5"/>
+      <c r="BU5"/>
+      <c r="BV5"/>
+      <c r="BW5"/>
+      <c r="BX5"/>
+      <c r="BY5"/>
+      <c r="BZ5"/>
+      <c r="CA5"/>
+      <c r="CB5"/>
+      <c r="CC5"/>
+      <c r="CD5"/>
+      <c r="CE5"/>
+      <c r="CF5"/>
+      <c r="CG5"/>
+      <c r="CH5"/>
+      <c r="CI5"/>
+      <c r="CJ5"/>
+      <c r="CK5"/>
+      <c r="CL5"/>
+      <c r="CM5"/>
+      <c r="CN5"/>
+      <c r="CO5"/>
+      <c r="CP5"/>
+      <c r="CQ5"/>
+      <c r="CR5"/>
+      <c r="CS5"/>
+      <c r="CT5"/>
+      <c r="CU5"/>
+    </row>
+    <row r="6" spans="1:99" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C6" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E6" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="N6" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+      <c r="S6"/>
+      <c r="T6"/>
+      <c r="U6"/>
+      <c r="V6"/>
+      <c r="W6"/>
+      <c r="X6"/>
+      <c r="Y6"/>
+      <c r="Z6"/>
+      <c r="AA6"/>
+      <c r="AB6"/>
+      <c r="AC6"/>
+      <c r="AD6"/>
+      <c r="AE6"/>
+      <c r="AF6"/>
+      <c r="AG6"/>
+      <c r="AH6"/>
+      <c r="AI6"/>
+      <c r="AJ6"/>
+      <c r="AK6"/>
+      <c r="AL6"/>
+      <c r="AM6"/>
+      <c r="AN6"/>
+      <c r="AO6"/>
+      <c r="AP6"/>
+      <c r="AQ6"/>
+      <c r="AR6"/>
+      <c r="AS6"/>
+      <c r="AT6"/>
+      <c r="AU6"/>
+      <c r="AV6"/>
+      <c r="AW6"/>
+      <c r="AX6"/>
+      <c r="AY6"/>
+      <c r="AZ6"/>
+      <c r="BA6"/>
+      <c r="BB6"/>
+      <c r="BC6"/>
+      <c r="BD6"/>
+      <c r="BE6"/>
+      <c r="BF6"/>
+      <c r="BG6"/>
+      <c r="BH6"/>
+      <c r="BI6"/>
+      <c r="BJ6"/>
+      <c r="BK6"/>
+      <c r="BL6"/>
+      <c r="BM6"/>
+      <c r="BN6"/>
+      <c r="BO6"/>
+      <c r="BP6"/>
+      <c r="BQ6"/>
+      <c r="BR6"/>
+      <c r="BS6"/>
+      <c r="BT6"/>
+      <c r="BU6"/>
+      <c r="BV6"/>
+      <c r="BW6"/>
+      <c r="BX6"/>
+      <c r="BY6"/>
+      <c r="BZ6"/>
+      <c r="CA6"/>
+      <c r="CB6"/>
+      <c r="CC6"/>
+      <c r="CD6"/>
+      <c r="CE6"/>
+      <c r="CF6"/>
+      <c r="CG6"/>
+      <c r="CH6"/>
+      <c r="CI6"/>
+      <c r="CJ6"/>
+      <c r="CK6"/>
+      <c r="CL6"/>
+      <c r="CM6"/>
+      <c r="CN6"/>
+      <c r="CO6"/>
+      <c r="CP6"/>
+      <c r="CQ6"/>
+      <c r="CR6"/>
+      <c r="CS6"/>
+      <c r="CT6"/>
+      <c r="CU6"/>
+    </row>
+    <row r="7" spans="1:99" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="19">
+        <v>1.9279999999999999</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="31">
+        <v>1000</v>
+      </c>
+      <c r="F7" s="31">
+        <v>4000</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="17">
+        <v>160000</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="28">
+        <v>9.3800000000000003E-5</v>
+      </c>
+      <c r="K7" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="35">
+        <v>2660</v>
+      </c>
+      <c r="M7" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="26">
+        <v>2660</v>
+      </c>
+      <c r="O7" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
+      <c r="U7"/>
+      <c r="V7"/>
+      <c r="W7"/>
+      <c r="X7"/>
+      <c r="Y7"/>
+      <c r="Z7"/>
+      <c r="AA7"/>
+      <c r="AB7"/>
+      <c r="AC7"/>
+      <c r="AD7"/>
+      <c r="AE7"/>
+      <c r="AF7"/>
+      <c r="AG7"/>
+      <c r="AH7"/>
+      <c r="AI7"/>
+      <c r="AJ7"/>
+      <c r="AK7"/>
+      <c r="AL7"/>
+      <c r="AM7"/>
+      <c r="AN7"/>
+      <c r="AO7"/>
+      <c r="AP7"/>
+      <c r="AQ7"/>
+      <c r="AR7"/>
+      <c r="AS7"/>
+      <c r="AT7"/>
+      <c r="AU7"/>
+      <c r="AV7"/>
+      <c r="AW7"/>
+      <c r="AX7"/>
+      <c r="AY7"/>
+      <c r="AZ7"/>
+      <c r="BA7"/>
+      <c r="BB7"/>
+      <c r="BC7"/>
+      <c r="BD7"/>
+      <c r="BE7"/>
+      <c r="BF7"/>
+      <c r="BG7"/>
+      <c r="BH7"/>
+      <c r="BI7"/>
+      <c r="BJ7"/>
+      <c r="BK7"/>
+      <c r="BL7"/>
+      <c r="BM7"/>
+      <c r="BN7"/>
+      <c r="BO7"/>
+      <c r="BP7"/>
+      <c r="BQ7"/>
+      <c r="BR7"/>
+      <c r="BS7"/>
+      <c r="BT7"/>
+      <c r="BU7"/>
+      <c r="BV7"/>
+      <c r="BW7"/>
+      <c r="BX7"/>
+      <c r="BY7"/>
+      <c r="BZ7"/>
+      <c r="CA7"/>
+      <c r="CB7"/>
+      <c r="CC7"/>
+      <c r="CD7"/>
+      <c r="CE7"/>
+      <c r="CF7"/>
+      <c r="CG7"/>
+      <c r="CH7"/>
+      <c r="CI7"/>
+      <c r="CJ7"/>
+      <c r="CK7"/>
+      <c r="CL7"/>
+      <c r="CM7"/>
+      <c r="CN7"/>
+      <c r="CO7"/>
+      <c r="CP7"/>
+      <c r="CQ7"/>
+      <c r="CR7"/>
+      <c r="CS7"/>
+      <c r="CT7"/>
+      <c r="CU7"/>
+    </row>
+    <row r="8" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="19">
+        <v>1.9370000000000001</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="31">
+        <v>500</v>
+      </c>
+      <c r="F8" s="31">
+        <v>1000</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="17">
+        <v>22000</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="28">
+        <v>9.3800000000000003E-5</v>
+      </c>
+      <c r="K8" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="35">
+        <v>990</v>
+      </c>
+      <c r="M8" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" s="26">
+        <v>990</v>
+      </c>
+      <c r="O8" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="P8"/>
+      <c r="Q8"/>
+      <c r="R8"/>
+      <c r="S8"/>
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8"/>
+      <c r="W8"/>
+      <c r="X8"/>
+      <c r="Y8"/>
+      <c r="Z8"/>
+      <c r="AA8"/>
+      <c r="AB8"/>
+      <c r="AC8"/>
+      <c r="AD8"/>
+      <c r="AE8"/>
+      <c r="AF8"/>
+      <c r="AG8"/>
+      <c r="AH8"/>
+      <c r="AI8"/>
+      <c r="AJ8"/>
+      <c r="AK8"/>
+      <c r="AL8"/>
+      <c r="AM8"/>
+      <c r="AN8"/>
+      <c r="AO8"/>
+      <c r="AP8"/>
+      <c r="AQ8"/>
+      <c r="AR8"/>
+      <c r="AS8"/>
+      <c r="AT8"/>
+      <c r="AU8"/>
+      <c r="AV8"/>
+      <c r="AW8"/>
+      <c r="AX8"/>
+      <c r="AY8"/>
+      <c r="AZ8"/>
+      <c r="BA8"/>
+      <c r="BB8"/>
+      <c r="BC8"/>
+      <c r="BD8"/>
+      <c r="BE8"/>
+      <c r="BF8"/>
+      <c r="BG8"/>
+      <c r="BH8"/>
+      <c r="BI8"/>
+      <c r="BJ8"/>
+      <c r="BK8"/>
+      <c r="BL8"/>
+      <c r="BM8"/>
+      <c r="BN8"/>
+      <c r="BO8"/>
+      <c r="BP8"/>
+      <c r="BQ8"/>
+      <c r="BR8"/>
+      <c r="BS8"/>
+      <c r="BT8"/>
+      <c r="BU8"/>
+      <c r="BV8"/>
+      <c r="BW8"/>
+      <c r="BX8"/>
+      <c r="BY8"/>
+      <c r="BZ8"/>
+      <c r="CA8"/>
+      <c r="CB8"/>
+      <c r="CC8"/>
+      <c r="CD8"/>
+      <c r="CE8"/>
+      <c r="CF8"/>
+      <c r="CG8"/>
+      <c r="CH8"/>
+      <c r="CI8"/>
+      <c r="CJ8"/>
+      <c r="CK8"/>
+      <c r="CL8"/>
+      <c r="CM8"/>
+      <c r="CN8"/>
+      <c r="CO8"/>
+      <c r="CP8"/>
+      <c r="CQ8"/>
+      <c r="CR8"/>
+      <c r="CS8"/>
+      <c r="CT8"/>
+      <c r="CU8"/>
+    </row>
+    <row r="9" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="19">
+        <v>7.476</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="33">
+        <v>10</v>
+      </c>
+      <c r="F9" s="33">
+        <v>70</v>
+      </c>
+      <c r="G9" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="17">
+        <v>2600</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="28">
+        <v>9.3800000000000003E-5</v>
+      </c>
+      <c r="K9" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" s="37">
+        <v>40.24</v>
+      </c>
+      <c r="M9" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" s="30">
+        <v>40.24</v>
+      </c>
+      <c r="O9" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="P9"/>
+      <c r="Q9"/>
+      <c r="R9"/>
+      <c r="S9"/>
+      <c r="T9"/>
+      <c r="U9"/>
+      <c r="V9"/>
+      <c r="W9"/>
+      <c r="X9"/>
+      <c r="Y9"/>
+      <c r="Z9"/>
+      <c r="AA9"/>
+      <c r="AB9"/>
+      <c r="AC9"/>
+      <c r="AD9"/>
+      <c r="AE9"/>
+      <c r="AF9"/>
+      <c r="AG9"/>
+      <c r="AH9"/>
+      <c r="AI9"/>
+      <c r="AJ9"/>
+      <c r="AK9"/>
+      <c r="AL9"/>
+      <c r="AM9"/>
+      <c r="AN9"/>
+      <c r="AO9"/>
+      <c r="AP9"/>
+      <c r="AQ9"/>
+      <c r="AR9"/>
+      <c r="AS9"/>
+      <c r="AT9"/>
+      <c r="AU9"/>
+      <c r="AV9"/>
+      <c r="AW9"/>
+      <c r="AX9"/>
+      <c r="AY9"/>
+      <c r="AZ9"/>
+      <c r="BA9"/>
+      <c r="BB9"/>
+      <c r="BC9"/>
+      <c r="BD9"/>
+      <c r="BE9"/>
+      <c r="BF9"/>
+      <c r="BG9"/>
+      <c r="BH9"/>
+      <c r="BI9"/>
+      <c r="BJ9"/>
+      <c r="BK9"/>
+      <c r="BL9"/>
+      <c r="BM9"/>
+      <c r="BN9"/>
+      <c r="BO9"/>
+      <c r="BP9"/>
+      <c r="BQ9"/>
+      <c r="BR9"/>
+      <c r="BS9"/>
+      <c r="BT9"/>
+      <c r="BU9"/>
+      <c r="BV9"/>
+      <c r="BW9"/>
+      <c r="BX9"/>
+      <c r="BY9"/>
+      <c r="BZ9"/>
+      <c r="CA9"/>
+      <c r="CB9"/>
+      <c r="CC9"/>
+      <c r="CD9"/>
+      <c r="CE9"/>
+      <c r="CF9"/>
+      <c r="CG9"/>
+      <c r="CH9"/>
+      <c r="CI9"/>
+      <c r="CJ9"/>
+      <c r="CK9"/>
+      <c r="CL9"/>
+      <c r="CM9"/>
+      <c r="CN9"/>
+      <c r="CO9"/>
+      <c r="CP9"/>
+      <c r="CQ9"/>
+      <c r="CR9"/>
+      <c r="CS9"/>
+      <c r="CT9"/>
+      <c r="CU9"/>
+    </row>
+    <row r="10" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="19">
+        <v>25.783000000000001</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="33">
+        <v>8.5</v>
+      </c>
+      <c r="F10" s="33">
+        <v>10</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="19">
+        <v>6.5</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="28">
+        <v>9.3800000000000003E-5</v>
+      </c>
+      <c r="K10" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" s="37">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="M10" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="N10" s="30">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="O10" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+      <c r="T10"/>
+      <c r="U10"/>
+      <c r="V10"/>
+      <c r="W10"/>
+      <c r="X10"/>
+      <c r="Y10"/>
+      <c r="Z10"/>
+      <c r="AA10"/>
+      <c r="AB10"/>
+      <c r="AC10"/>
+      <c r="AD10"/>
+      <c r="AE10"/>
+      <c r="AF10"/>
+      <c r="AG10"/>
+      <c r="AH10"/>
+      <c r="AI10"/>
+      <c r="AJ10"/>
+      <c r="AK10"/>
+      <c r="AL10"/>
+      <c r="AM10"/>
+      <c r="AN10"/>
+      <c r="AO10"/>
+      <c r="AP10"/>
+      <c r="AQ10"/>
+      <c r="AR10"/>
+      <c r="AS10"/>
+      <c r="AT10"/>
+      <c r="AU10"/>
+      <c r="AV10"/>
+      <c r="AW10"/>
+      <c r="AX10"/>
+      <c r="AY10"/>
+      <c r="AZ10"/>
+      <c r="BA10"/>
+      <c r="BB10"/>
+      <c r="BC10"/>
+      <c r="BD10"/>
+      <c r="BE10"/>
+      <c r="BF10"/>
+      <c r="BG10"/>
+      <c r="BH10"/>
+      <c r="BI10"/>
+      <c r="BJ10"/>
+      <c r="BK10"/>
+      <c r="BL10"/>
+      <c r="BM10"/>
+      <c r="BN10"/>
+      <c r="BO10"/>
+      <c r="BP10"/>
+      <c r="BQ10"/>
+      <c r="BR10"/>
+      <c r="BS10"/>
+      <c r="BT10"/>
+      <c r="BU10"/>
+      <c r="BV10"/>
+      <c r="BW10"/>
+      <c r="BX10"/>
+      <c r="BY10"/>
+      <c r="BZ10"/>
+      <c r="CA10"/>
+      <c r="CB10"/>
+      <c r="CC10"/>
+      <c r="CD10"/>
+      <c r="CE10"/>
+      <c r="CF10"/>
+      <c r="CG10"/>
+      <c r="CH10"/>
+      <c r="CI10"/>
+      <c r="CJ10"/>
+      <c r="CK10"/>
+      <c r="CL10"/>
+      <c r="CM10"/>
+      <c r="CN10"/>
+      <c r="CO10"/>
+      <c r="CP10"/>
+      <c r="CQ10"/>
+      <c r="CR10"/>
+      <c r="CS10"/>
+      <c r="CT10"/>
+      <c r="CU10"/>
+    </row>
+    <row r="11" spans="1:99" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>20000</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+    </row>
+    <row r="12" spans="1:99" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
+      <c r="B12" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" spans="1:99" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="B13" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="L13" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="M13" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="N13" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="O13" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:99" s="2" customFormat="1" ht="33.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="21">
+        <v>4200000</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="31">
+        <v>1400000</v>
+      </c>
+      <c r="F14" s="31">
+        <v>60000000</v>
+      </c>
+      <c r="G14" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" s="10">
+        <v>2860000</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="M14" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="N14" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O14" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
+      <c r="S14"/>
+      <c r="T14"/>
+      <c r="U14"/>
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14"/>
+      <c r="Y14"/>
+      <c r="Z14"/>
+      <c r="AA14"/>
+      <c r="AB14"/>
+      <c r="AC14"/>
+      <c r="AD14"/>
+      <c r="AE14"/>
+      <c r="AF14"/>
+      <c r="AG14"/>
+      <c r="AH14"/>
+      <c r="AI14"/>
+      <c r="AJ14"/>
+      <c r="AK14"/>
+      <c r="AL14"/>
+      <c r="AM14"/>
+      <c r="AN14"/>
+      <c r="AO14"/>
+      <c r="AP14"/>
+      <c r="AQ14"/>
+      <c r="AR14"/>
+      <c r="AS14"/>
+      <c r="AT14"/>
+      <c r="AU14"/>
+      <c r="AV14"/>
+      <c r="AW14"/>
+      <c r="AX14"/>
+      <c r="AY14"/>
+      <c r="AZ14"/>
+      <c r="BA14"/>
+      <c r="BB14"/>
+      <c r="BC14"/>
+      <c r="BD14"/>
+      <c r="BE14"/>
+      <c r="BF14"/>
+      <c r="BG14"/>
+      <c r="BH14"/>
+      <c r="BI14"/>
+      <c r="BJ14"/>
+      <c r="BK14"/>
+      <c r="BL14"/>
+      <c r="BM14"/>
+      <c r="BN14"/>
+      <c r="BO14"/>
+      <c r="BP14"/>
+      <c r="BQ14"/>
+      <c r="BR14"/>
+      <c r="BS14"/>
+      <c r="BT14"/>
+      <c r="BU14"/>
+      <c r="BV14"/>
+      <c r="BW14"/>
+      <c r="BX14"/>
+      <c r="BY14"/>
+      <c r="BZ14"/>
+      <c r="CA14"/>
+      <c r="CB14"/>
+      <c r="CC14"/>
+      <c r="CD14"/>
+      <c r="CE14"/>
+      <c r="CF14"/>
+      <c r="CG14"/>
+      <c r="CH14"/>
+      <c r="CI14"/>
+      <c r="CJ14"/>
+      <c r="CK14"/>
+      <c r="CL14"/>
+      <c r="CM14"/>
+      <c r="CN14"/>
+      <c r="CO14"/>
+      <c r="CP14"/>
+      <c r="CQ14"/>
+      <c r="CR14"/>
+      <c r="CS14"/>
+      <c r="CT14"/>
+      <c r="CU14"/>
+    </row>
+    <row r="15" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15" s="35">
+        <v>30000000</v>
+      </c>
+      <c r="M15" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="N15" s="26">
+        <v>30000000</v>
+      </c>
+      <c r="O15" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="P15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15"/>
+      <c r="S15"/>
+      <c r="T15"/>
+      <c r="U15"/>
+      <c r="V15"/>
+      <c r="W15"/>
+      <c r="X15"/>
+      <c r="Y15"/>
+      <c r="Z15"/>
+      <c r="AA15"/>
+      <c r="AB15"/>
+      <c r="AC15"/>
+      <c r="AD15"/>
+      <c r="AE15"/>
+      <c r="AF15"/>
+      <c r="AG15"/>
+      <c r="AH15"/>
+      <c r="AI15"/>
+      <c r="AJ15"/>
+      <c r="AK15"/>
+      <c r="AL15"/>
+      <c r="AM15"/>
+      <c r="AN15"/>
+      <c r="AO15"/>
+      <c r="AP15"/>
+      <c r="AQ15"/>
+      <c r="AR15"/>
+      <c r="AS15"/>
+      <c r="AT15"/>
+      <c r="AU15"/>
+      <c r="AV15"/>
+      <c r="AW15"/>
+      <c r="AX15"/>
+      <c r="AY15"/>
+      <c r="AZ15"/>
+      <c r="BA15"/>
+      <c r="BB15"/>
+      <c r="BC15"/>
+      <c r="BD15"/>
+      <c r="BE15"/>
+      <c r="BF15"/>
+      <c r="BG15"/>
+      <c r="BH15"/>
+      <c r="BI15"/>
+      <c r="BJ15"/>
+      <c r="BK15"/>
+      <c r="BL15"/>
+      <c r="BM15"/>
+      <c r="BN15"/>
+      <c r="BO15"/>
+      <c r="BP15"/>
+      <c r="BQ15"/>
+      <c r="BR15"/>
+      <c r="BS15"/>
+      <c r="BT15"/>
+      <c r="BU15"/>
+      <c r="BV15"/>
+      <c r="BW15"/>
+      <c r="BX15"/>
+      <c r="BY15"/>
+      <c r="BZ15"/>
+      <c r="CA15"/>
+      <c r="CB15"/>
+      <c r="CC15"/>
+      <c r="CD15"/>
+      <c r="CE15"/>
+      <c r="CF15"/>
+      <c r="CG15"/>
+      <c r="CH15"/>
+      <c r="CI15"/>
+      <c r="CJ15"/>
+      <c r="CK15"/>
+      <c r="CL15"/>
+      <c r="CM15"/>
+      <c r="CN15"/>
+      <c r="CO15"/>
+      <c r="CP15"/>
+      <c r="CQ15"/>
+      <c r="CR15"/>
+      <c r="CS15"/>
+      <c r="CT15"/>
+      <c r="CU15"/>
+    </row>
+    <row r="16" spans="1:99" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="12"/>
+      <c r="B16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="L16" s="35">
+        <v>10000000</v>
+      </c>
+      <c r="M16" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="N16" s="26">
+        <v>50000000</v>
+      </c>
+      <c r="O16" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="P16"/>
+      <c r="Q16" s="15"/>
+      <c r="R16"/>
+      <c r="S16"/>
+      <c r="T16"/>
+      <c r="U16"/>
+      <c r="V16"/>
+      <c r="W16"/>
+      <c r="X16"/>
+      <c r="Y16"/>
+      <c r="Z16"/>
+      <c r="AA16"/>
+      <c r="AB16"/>
+      <c r="AC16"/>
+      <c r="AD16"/>
+      <c r="AE16"/>
+      <c r="AF16"/>
+      <c r="AG16"/>
+      <c r="AH16"/>
+      <c r="AI16"/>
+      <c r="AJ16"/>
+      <c r="AK16"/>
+      <c r="AL16"/>
+      <c r="AM16"/>
+      <c r="AN16"/>
+      <c r="AO16"/>
+      <c r="AP16"/>
+      <c r="AQ16"/>
+      <c r="AR16"/>
+      <c r="AS16"/>
+      <c r="AT16"/>
+      <c r="AU16"/>
+      <c r="AV16"/>
+      <c r="AW16"/>
+      <c r="AX16"/>
+      <c r="AY16"/>
+      <c r="AZ16"/>
+      <c r="BA16"/>
+      <c r="BB16"/>
+      <c r="BC16"/>
+      <c r="BD16"/>
+      <c r="BE16"/>
+      <c r="BF16"/>
+      <c r="BG16"/>
+      <c r="BH16"/>
+      <c r="BI16"/>
+      <c r="BJ16"/>
+      <c r="BK16"/>
+      <c r="BL16"/>
+      <c r="BM16"/>
+      <c r="BN16"/>
+      <c r="BO16"/>
+      <c r="BP16"/>
+      <c r="BQ16"/>
+      <c r="BR16"/>
+      <c r="BS16"/>
+      <c r="BT16"/>
+      <c r="BU16"/>
+      <c r="BV16"/>
+      <c r="BW16"/>
+      <c r="BX16"/>
+      <c r="BY16"/>
+      <c r="BZ16"/>
+      <c r="CA16"/>
+      <c r="CB16"/>
+      <c r="CC16"/>
+      <c r="CD16"/>
+      <c r="CE16"/>
+      <c r="CF16"/>
+      <c r="CG16"/>
+      <c r="CH16"/>
+      <c r="CI16"/>
+      <c r="CJ16"/>
+      <c r="CK16"/>
+      <c r="CL16"/>
+      <c r="CM16"/>
+      <c r="CN16"/>
+      <c r="CO16"/>
+      <c r="CP16"/>
+      <c r="CQ16"/>
+      <c r="CR16"/>
+      <c r="CS16"/>
+      <c r="CT16"/>
+      <c r="CU16"/>
+    </row>
+    <row r="17" spans="1:99" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="12"/>
+      <c r="B17" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="C17" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
+      <c r="E17" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="K17" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="L17" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="M17" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="N17" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="O17" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="P17"/>
+      <c r="Q17" s="15"/>
+      <c r="R17"/>
+      <c r="S17"/>
+      <c r="T17"/>
+      <c r="U17"/>
+      <c r="V17"/>
+      <c r="W17"/>
+      <c r="X17"/>
+      <c r="Y17"/>
+      <c r="Z17"/>
+      <c r="AA17"/>
+      <c r="AB17"/>
+      <c r="AC17"/>
+      <c r="AD17"/>
+      <c r="AE17"/>
+      <c r="AF17"/>
+      <c r="AG17"/>
+      <c r="AH17"/>
+      <c r="AI17"/>
+      <c r="AJ17"/>
+      <c r="AK17"/>
+      <c r="AL17"/>
+      <c r="AM17"/>
+      <c r="AN17"/>
+      <c r="AO17"/>
+      <c r="AP17"/>
+      <c r="AQ17"/>
+      <c r="AR17"/>
+      <c r="AS17"/>
+      <c r="AT17"/>
+      <c r="AU17"/>
+      <c r="AV17"/>
+      <c r="AW17"/>
+      <c r="AX17"/>
+      <c r="AY17"/>
+      <c r="AZ17"/>
+      <c r="BA17"/>
+      <c r="BB17"/>
+      <c r="BC17"/>
+      <c r="BD17"/>
+      <c r="BE17"/>
+      <c r="BF17"/>
+      <c r="BG17"/>
+      <c r="BH17"/>
+      <c r="BI17"/>
+      <c r="BJ17"/>
+      <c r="BK17"/>
+      <c r="BL17"/>
+      <c r="BM17"/>
+      <c r="BN17"/>
+      <c r="BO17"/>
+      <c r="BP17"/>
+      <c r="BQ17"/>
+      <c r="BR17"/>
+      <c r="BS17"/>
+      <c r="BT17"/>
+      <c r="BU17"/>
+      <c r="BV17"/>
+      <c r="BW17"/>
+      <c r="BX17"/>
+      <c r="BY17"/>
+      <c r="BZ17"/>
+      <c r="CA17"/>
+      <c r="CB17"/>
+      <c r="CC17"/>
+      <c r="CD17"/>
+      <c r="CE17"/>
+      <c r="CF17"/>
+      <c r="CG17"/>
+      <c r="CH17"/>
+      <c r="CI17"/>
+      <c r="CJ17"/>
+      <c r="CK17"/>
+      <c r="CL17"/>
+      <c r="CM17"/>
+      <c r="CN17"/>
+      <c r="CO17"/>
+      <c r="CP17"/>
+      <c r="CQ17"/>
+      <c r="CR17"/>
+      <c r="CS17"/>
+      <c r="CT17"/>
+      <c r="CU17"/>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1000000</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1.9279999999999999</v>
+    <row r="18" spans="1:99" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="17">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="33">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F18" s="33">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G18" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J18" s="9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L18" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="M18" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="N18" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="O18" s="29" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="2" t="s">
+    <row r="19" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3">
-        <v>1000000</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="C19" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L19" s="37">
+        <v>1.95</v>
+      </c>
+      <c r="M19" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="N19" s="30">
+        <v>1.95</v>
+      </c>
+      <c r="O19" s="29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:99" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="2">
-        <v>1.9370000000000001</v>
+      <c r="C20" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L20" s="37">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M20" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="N20" s="26">
+        <v>9.0000000000000006E-5</v>
+      </c>
+      <c r="O20" s="29" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="2" t="s">
+    <row r="21" spans="1:99" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11"/>
+      <c r="B21" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="J21" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="K21" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="L21" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="M21" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="N21" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="O21" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:99" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3">
-        <v>1000000</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="B22" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="2">
-        <v>7.476</v>
-      </c>
+      <c r="C22" s="25">
+        <v>10</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="33">
+        <v>0.5</v>
+      </c>
+      <c r="F22" s="33">
+        <v>1.25</v>
+      </c>
+      <c r="G22" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J22" s="3"/>
+      <c r="L22" s="37">
+        <v>0.96</v>
+      </c>
+      <c r="M22" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="N22" s="30">
+        <v>0.96</v>
+      </c>
+      <c r="O22" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="P22"/>
+      <c r="Q22"/>
+      <c r="R22"/>
+      <c r="S22"/>
+      <c r="T22"/>
+      <c r="U22"/>
+      <c r="V22"/>
+      <c r="W22"/>
+      <c r="X22"/>
+      <c r="Y22"/>
+      <c r="Z22"/>
+      <c r="AA22"/>
+      <c r="AB22"/>
+      <c r="AC22"/>
+      <c r="AD22"/>
+      <c r="AE22"/>
+      <c r="AF22"/>
+      <c r="AG22"/>
+      <c r="AH22"/>
+      <c r="AI22"/>
+      <c r="AJ22"/>
+      <c r="AK22"/>
+      <c r="AL22"/>
+      <c r="AM22"/>
+      <c r="AN22"/>
+      <c r="AO22"/>
+      <c r="AP22"/>
+      <c r="AQ22"/>
+      <c r="AR22"/>
+      <c r="AS22"/>
+      <c r="AT22"/>
+      <c r="AU22"/>
+      <c r="AV22"/>
+      <c r="AW22"/>
+      <c r="AX22"/>
+      <c r="AY22"/>
+      <c r="AZ22"/>
+      <c r="BA22"/>
+      <c r="BB22"/>
+      <c r="BC22"/>
+      <c r="BD22"/>
+      <c r="BE22"/>
+      <c r="BF22"/>
+      <c r="BG22"/>
+      <c r="BH22"/>
+      <c r="BI22"/>
+      <c r="BJ22"/>
+      <c r="BK22"/>
+      <c r="BL22"/>
+      <c r="BM22"/>
+      <c r="BN22"/>
+      <c r="BO22"/>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="2" t="s">
+    <row r="23" spans="1:99" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3">
-        <v>1000000</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="B23" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="2">
-        <v>25.783000000000001</v>
+      <c r="C23" s="41">
+        <v>0.02</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="46">
+        <v>0.01</v>
+      </c>
+      <c r="F23" s="44">
+        <v>0.05</v>
+      </c>
+      <c r="G23" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="I23" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="L23" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="M23" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="N23" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="O23" s="30" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="24" spans="1:99" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="11"/>
+      <c r="B24" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="H24" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="I24" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="J24" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="K24" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="L24" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="M24" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="N24" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="O24" s="16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:99" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B25" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1">
-        <v>20000</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="1">
-        <v>10000000</v>
-      </c>
-      <c r="G6" t="s">
-        <v>29</v>
-      </c>
+      <c r="C25" s="39">
+        <v>20</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="34"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="L25" s="33">
+        <v>0.41</v>
+      </c>
+      <c r="M25" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="N25" s="25">
+        <v>11.5</v>
+      </c>
+      <c r="O25" s="25"/>
+      <c r="P25"/>
+      <c r="Q25"/>
+      <c r="R25"/>
+      <c r="S25"/>
+      <c r="T25"/>
+      <c r="U25"/>
+      <c r="V25"/>
+      <c r="W25"/>
+      <c r="X25"/>
+      <c r="Y25"/>
+      <c r="Z25"/>
+      <c r="AA25"/>
+      <c r="AB25"/>
+      <c r="AC25"/>
+      <c r="AD25"/>
+      <c r="AE25"/>
+      <c r="AF25"/>
+      <c r="AG25"/>
+      <c r="AH25"/>
+      <c r="AI25"/>
+      <c r="AJ25"/>
+      <c r="AK25"/>
+      <c r="AL25"/>
+      <c r="AM25"/>
+      <c r="AN25"/>
+      <c r="AO25"/>
+      <c r="AP25"/>
+      <c r="AQ25"/>
+      <c r="AR25"/>
+      <c r="AS25"/>
+      <c r="AT25"/>
+      <c r="AU25"/>
+      <c r="AV25"/>
+      <c r="AW25"/>
+      <c r="AX25"/>
+      <c r="AY25"/>
+      <c r="AZ25"/>
+      <c r="BA25"/>
+      <c r="BB25"/>
+      <c r="BC25"/>
+      <c r="BD25"/>
+      <c r="BE25"/>
+      <c r="BF25"/>
+      <c r="BG25"/>
+      <c r="BH25"/>
+      <c r="BI25"/>
+      <c r="BJ25"/>
+      <c r="BK25"/>
+      <c r="BL25"/>
+      <c r="BM25"/>
+      <c r="BN25"/>
+      <c r="BO25"/>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3">
-        <v>4200000</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>27</v>
+    <row r="26" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="3">
-        <v>20</v>
+    <row r="27" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
rxn rate names match excel spreadsheet
</commit_message>
<xml_diff>
--- a/rxns_table.xlsx
+++ b/rxns_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD_2023\CaMKII_hexa_bgnl_to_mcell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E7EA75-C412-41F4-93C7-373E5DA996DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3590B8F8-F975-49CC-956B-112E85E5906F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="1260" windowWidth="19420" windowHeight="10420" xr2:uid="{4B4FB280-5B08-406D-B059-D87F72317E26}"/>
   </bookViews>
@@ -117,21 +117,12 @@
     <t>CaMKII T286 phosphorylation</t>
   </si>
   <si>
-    <t>K_P_CaMKII286</t>
-  </si>
-  <si>
     <t>CaMKII T306 phosphorylation</t>
   </si>
   <si>
-    <t>K_P_CaMKII306</t>
-  </si>
-  <si>
     <t>CaMKII dephosphorylation by PP1</t>
   </si>
   <si>
-    <t>Kcat</t>
-  </si>
-  <si>
     <t>Stefan et al., 2012; Pharris et al., 2020</t>
   </si>
   <si>
@@ -238,13 +229,22 @@
   </si>
   <si>
     <t>CaMKII</t>
+  </si>
+  <si>
+    <t>k_P_CaMKII286</t>
+  </si>
+  <si>
+    <t>k_P_CaMKII306</t>
+  </si>
+  <si>
+    <t>k_cat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -424,12 +424,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <b/>
@@ -876,7 +870,7 @@
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="39" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="18" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
@@ -1281,7 +1275,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B603CBE9-61C1-43B8-82FF-7D32E551985B}">
   <dimension ref="A1:CU27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -1310,43 +1304,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C1" s="38" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D1" s="38" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="38" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F1" s="38" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G1" s="38" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="38" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I1" s="38" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="38" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K1" s="38" t="s">
         <v>2</v>
       </c>
       <c r="L1" s="38" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="M1" s="38" t="s">
         <v>2</v>
       </c>
       <c r="N1" s="38" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="O1" s="38" t="s">
         <v>2</v>
@@ -1354,16 +1348,16 @@
     </row>
     <row r="2" spans="1:99" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C2" s="17">
         <v>1000000</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E2" s="31">
         <v>25000000</v>
@@ -1372,31 +1366,31 @@
         <v>260000000</v>
       </c>
       <c r="G2" s="32" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H2" s="17">
         <v>770000000</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J2" s="26">
         <v>32200000000</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L2" s="35">
         <v>100000000</v>
       </c>
       <c r="M2" s="36" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N2" s="26">
         <v>100000000</v>
       </c>
       <c r="O2" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="P2"/>
       <c r="Q2"/>
@@ -1486,13 +1480,13 @@
     <row r="3" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C3" s="17">
         <v>1000000</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E3" s="31">
         <v>50000000</v>
@@ -1501,31 +1495,31 @@
         <v>300000000</v>
       </c>
       <c r="G3" s="32" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H3" s="17">
         <v>32000000000</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J3" s="26">
         <v>32200000000</v>
       </c>
       <c r="K3" s="27" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L3" s="35">
         <v>150000000</v>
       </c>
       <c r="M3" s="36" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N3" s="26">
         <v>150000000</v>
       </c>
       <c r="O3" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="P3"/>
       <c r="Q3"/>
@@ -1615,13 +1609,13 @@
     <row r="4" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C4" s="17">
         <v>1000000</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E4" s="31">
         <v>1200000</v>
@@ -1630,31 +1624,31 @@
         <v>9600000</v>
       </c>
       <c r="G4" s="32" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H4" s="17">
         <v>84000000</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J4" s="26">
         <v>322000000</v>
       </c>
       <c r="K4" s="27" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L4" s="35">
         <v>4000000</v>
       </c>
       <c r="M4" s="36" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N4" s="26">
         <v>4000000</v>
       </c>
       <c r="O4" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="P4"/>
       <c r="Q4"/>
@@ -1744,13 +1738,13 @@
     <row r="5" spans="1:99" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C5" s="17">
         <v>1000000</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E5" s="31">
         <v>5000000</v>
@@ -1759,31 +1753,31 @@
         <v>25000000</v>
       </c>
       <c r="G5" s="32" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H5" s="17">
         <v>250000000</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J5" s="26">
         <v>322000000</v>
       </c>
       <c r="K5" s="27" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L5" s="35">
         <v>10000000</v>
       </c>
       <c r="M5" s="36" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N5" s="26">
         <v>10000000</v>
       </c>
       <c r="O5" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="P5"/>
       <c r="Q5"/>
@@ -1872,46 +1866,46 @@
     </row>
     <row r="6" spans="1:99" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B6" s="38" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D6" s="38" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G6" s="38" t="s">
         <v>2</v>
       </c>
       <c r="H6" s="38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I6" s="38" t="s">
         <v>2</v>
       </c>
       <c r="J6" s="38" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K6" s="38" t="s">
         <v>2</v>
       </c>
       <c r="L6" s="38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="M6" s="38" t="s">
         <v>2</v>
       </c>
       <c r="N6" s="38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="O6" s="38" t="s">
         <v>2</v>
@@ -2004,13 +1998,13 @@
     <row r="7" spans="1:99" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C7" s="19">
         <v>1.9279999999999999</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E7" s="31">
         <v>1000</v>
@@ -2019,31 +2013,31 @@
         <v>4000</v>
       </c>
       <c r="G7" s="32" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H7" s="17">
         <v>160000</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J7" s="28">
         <v>9.3800000000000003E-5</v>
       </c>
       <c r="K7" s="27" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L7" s="35">
         <v>2660</v>
       </c>
       <c r="M7" s="36" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N7" s="26">
         <v>2660</v>
       </c>
       <c r="O7" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="P7"/>
       <c r="Q7"/>
@@ -2133,13 +2127,13 @@
     <row r="8" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C8" s="19">
         <v>1.9370000000000001</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E8" s="31">
         <v>500</v>
@@ -2148,31 +2142,31 @@
         <v>1000</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H8" s="17">
         <v>22000</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J8" s="28">
         <v>9.3800000000000003E-5</v>
       </c>
       <c r="K8" s="27" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L8" s="35">
         <v>990</v>
       </c>
       <c r="M8" s="36" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N8" s="26">
         <v>990</v>
       </c>
       <c r="O8" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="P8"/>
       <c r="Q8"/>
@@ -2262,13 +2256,13 @@
     <row r="9" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C9" s="19">
         <v>7.476</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E9" s="33">
         <v>10</v>
@@ -2277,31 +2271,31 @@
         <v>70</v>
       </c>
       <c r="G9" s="32" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H9" s="17">
         <v>2600</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J9" s="28">
         <v>9.3800000000000003E-5</v>
       </c>
       <c r="K9" s="27" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L9" s="37">
         <v>40.24</v>
       </c>
       <c r="M9" s="36" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N9" s="30">
         <v>40.24</v>
       </c>
       <c r="O9" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="P9"/>
       <c r="Q9"/>
@@ -2391,13 +2385,13 @@
     <row r="10" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C10" s="19">
         <v>25.783000000000001</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E10" s="33">
         <v>8.5</v>
@@ -2406,31 +2400,31 @@
         <v>10</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H10" s="19">
         <v>6.5</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J10" s="28">
         <v>9.3800000000000003E-5</v>
       </c>
       <c r="K10" s="27" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L10" s="37">
         <v>9.3000000000000007</v>
       </c>
       <c r="M10" s="36" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N10" s="30">
         <v>9.3000000000000007</v>
       </c>
       <c r="O10" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="P10"/>
       <c r="Q10"/>
@@ -2528,7 +2522,7 @@
         <v>20000</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="5"/>
@@ -2546,7 +2540,7 @@
         <v>10000000</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="5"/>
@@ -2558,43 +2552,43 @@
     <row r="13" spans="1:99" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="38" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D13" s="38" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="38" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F13" s="38" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G13" s="38" t="s">
         <v>2</v>
       </c>
       <c r="H13" s="38" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I13" s="38" t="s">
         <v>2</v>
       </c>
       <c r="J13" s="38" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K13" s="38" t="s">
         <v>2</v>
       </c>
       <c r="L13" s="38" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="M13" s="38" t="s">
         <v>2</v>
       </c>
       <c r="N13" s="38" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="O13" s="38" t="s">
         <v>2</v>
@@ -2602,7 +2596,7 @@
     </row>
     <row r="14" spans="1:99" s="2" customFormat="1" ht="33.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>6</v>
@@ -2611,7 +2605,7 @@
         <v>4200000</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E14" s="31">
         <v>1400000</v>
@@ -2620,31 +2614,31 @@
         <v>60000000</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J14" s="10">
         <v>2860000</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L14" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="M14" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="N14" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="O14" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="P14"/>
       <c r="Q14"/>
@@ -2734,46 +2728,46 @@
     <row r="15" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L15" s="35">
         <v>30000000</v>
       </c>
       <c r="M15" s="36" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N15" s="26">
         <v>30000000</v>
       </c>
       <c r="O15" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="P15"/>
       <c r="Q15" s="15"/>
@@ -2863,46 +2857,46 @@
     <row r="16" spans="1:99" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12"/>
       <c r="B16" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F16" s="31" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G16" s="32" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L16" s="35">
         <v>10000000</v>
       </c>
       <c r="M16" s="36" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N16" s="26">
         <v>50000000</v>
       </c>
       <c r="O16" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="P16"/>
       <c r="Q16" s="15"/>
@@ -2995,40 +2989,40 @@
         <v>1</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D17" s="38" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F17" s="38" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G17" s="38" t="s">
         <v>2</v>
       </c>
       <c r="H17" s="38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I17" s="38" t="s">
         <v>2</v>
       </c>
       <c r="J17" s="38" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K17" s="38" t="s">
         <v>2</v>
       </c>
       <c r="L17" s="38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="M17" s="38" t="s">
         <v>2</v>
       </c>
       <c r="N17" s="38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="O17" s="38" t="s">
         <v>2</v>
@@ -3120,16 +3114,16 @@
     </row>
     <row r="18" spans="1:99" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C18" s="17">
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E18" s="33">
         <v>1.1000000000000001</v>
@@ -3138,31 +3132,31 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="G18" s="32" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J18" s="9">
         <v>1.1000000000000001</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L18" s="37" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M18" s="37" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N18" s="30" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="O18" s="29" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:99" x14ac:dyDescent="0.25">
@@ -3171,43 +3165,43 @@
         <v>7</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F19" s="33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G19" s="32" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="L19" s="37">
         <v>1.95</v>
       </c>
       <c r="M19" s="36" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N19" s="30">
         <v>1.95</v>
       </c>
       <c r="O19" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:99" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3216,85 +3210,85 @@
         <v>8</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F20" s="33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G20" s="32" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="L20" s="37">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="M20" s="36" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N20" s="26">
         <v>9.0000000000000006E-5</v>
       </c>
       <c r="O20" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:99" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11"/>
       <c r="B21" s="38" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D21" s="38" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F21" s="38" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G21" s="38" t="s">
         <v>2</v>
       </c>
       <c r="H21" s="38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I21" s="38" t="s">
         <v>2</v>
       </c>
       <c r="J21" s="38" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K21" s="38" t="s">
         <v>2</v>
       </c>
       <c r="L21" s="38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="M21" s="38" t="s">
         <v>2</v>
       </c>
       <c r="N21" s="38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="O21" s="38" t="s">
         <v>2</v>
@@ -3305,13 +3299,13 @@
         <v>9</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="C22" s="25">
         <v>10</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E22" s="33">
         <v>0.5</v>
@@ -3320,26 +3314,26 @@
         <v>1.25</v>
       </c>
       <c r="G22" s="32" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J22" s="3"/>
       <c r="L22" s="37">
         <v>0.96</v>
       </c>
       <c r="M22" s="36" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N22" s="30">
         <v>0.96</v>
       </c>
       <c r="O22" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="P22"/>
       <c r="Q22"/>
@@ -3396,16 +3390,16 @@
     </row>
     <row r="23" spans="1:99" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="C23" s="41">
         <v>0.02</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E23" s="46">
         <v>0.01</v>
@@ -3414,25 +3408,25 @@
         <v>0.05</v>
       </c>
       <c r="G23" s="45" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H23" s="42" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I23" s="43" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L23" s="37" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M23" s="37" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N23" s="30" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="O23" s="30" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:99" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3441,40 +3435,40 @@
         <v>1</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D24" s="38" t="s">
         <v>2</v>
       </c>
       <c r="E24" s="38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F24" s="38" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G24" s="38" t="s">
         <v>2</v>
       </c>
       <c r="H24" s="38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I24" s="38" t="s">
         <v>2</v>
       </c>
       <c r="J24" s="38" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K24" s="38" t="s">
         <v>2</v>
       </c>
       <c r="L24" s="38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="M24" s="38" t="s">
         <v>2</v>
       </c>
       <c r="N24" s="38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="O24" s="16" t="s">
         <v>2</v>
@@ -3482,16 +3476,16 @@
     </row>
     <row r="25" spans="1:99" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="C25" s="39">
         <v>20</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E25" s="34"/>
       <c r="F25" s="33"/>
@@ -3503,7 +3497,7 @@
         <v>0.41</v>
       </c>
       <c r="M25" s="36" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N25" s="25">
         <v>11.5</v>
@@ -3564,12 +3558,12 @@
     </row>
     <row r="26" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added domas rxns to excel table; plus reactions corrected with conditions explained after meeting w/ melanie
</commit_message>
<xml_diff>
--- a/rxns_table.xlsx
+++ b/rxns_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD_2023\CaMKII_hexa_bgnl_to_mcell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3590B8F8-F975-49CC-956B-112E85E5906F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B674CA7-6D22-4BCB-A652-53AEDFE8C568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="1260" windowWidth="19420" windowHeight="10420" xr2:uid="{4B4FB280-5B08-406D-B059-D87F72317E26}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4B4FB280-5B08-406D-B059-D87F72317E26}"/>
   </bookViews>
   <sheets>
     <sheet name="rxns_table" sheetId="1" r:id="rId1"/>
@@ -35,12 +35,34 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={67578144-E3EC-4152-8729-1B44EEC1002D}</author>
+    <author>tc={6F7C1780-1EE0-4B0C-B03B-9322192D7EC2}</author>
     <author>tc={B6F8C469-337C-40BE-B2DC-A13B6B68197A}</author>
     <author>Susana Roman</author>
     <author>tc={6C2818CD-9DCB-407F-A713-A0F009955982}</author>
   </authors>
   <commentList>
-    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{B6F8C469-337C-40BE-B2DC-A13B6B68197A}">
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{67578144-E3EC-4152-8729-1B44EEC1002D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Log10 converted to normal -&gt; from scheme 3 table 1
+Reply:
+    And ms to s</t>
+      </text>
+    </comment>
+    <comment ref="F7" authorId="1" shapeId="0" xr:uid="{6F7C1780-1EE0-4B0C-B03B-9322192D7EC2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Log10 converted to normal -&gt; from scheme 3 table 1
+Reply:
+    And ms to s</t>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="2" shapeId="0" xr:uid="{B6F8C469-337C-40BE-B2DC-A13B6B68197A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -48,7 +70,7 @@
     Not modelled currently; we specify different off rates depending on whether camkii is P or not.</t>
       </text>
     </comment>
-    <comment ref="L22" authorId="1" shapeId="0" xr:uid="{D783E934-AE8E-45F6-BF32-CFA5F3DEAB20}">
+    <comment ref="N22" authorId="3" shapeId="0" xr:uid="{D783E934-AE8E-45F6-BF32-CFA5F3DEAB20}">
       <text>
         <r>
           <rPr>
@@ -72,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N25" authorId="2" shapeId="0" xr:uid="{6C2818CD-9DCB-407F-A713-A0F009955982}">
+    <comment ref="P25" authorId="4" shapeId="0" xr:uid="{6C2818CD-9DCB-407F-A713-A0F009955982}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -85,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="55">
   <si>
     <t>Description</t>
   </si>
@@ -238,6 +260,18 @@
   </si>
   <si>
     <t>k_cat</t>
+  </si>
+  <si>
+    <t>Linkevicius et al., 2024</t>
+  </si>
+  <si>
+    <t>Linkevicius et al., 2025</t>
+  </si>
+  <si>
+    <t>Linkevicius et al., 2026</t>
+  </si>
+  <si>
+    <t>Linkevicius et al., 2027</t>
   </si>
 </sst>
 </file>
@@ -1262,10 +1296,22 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="F2" dT="2024-08-09T13:04:41.59" personId="{48458BD6-4CAC-498F-B01C-BB6F89FD41FA}" id="{67578144-E3EC-4152-8729-1B44EEC1002D}">
+    <text>Log10 converted to normal -&gt; from scheme 3 table 1</text>
+  </threadedComment>
+  <threadedComment ref="F2" dT="2024-08-09T13:04:59.39" personId="{48458BD6-4CAC-498F-B01C-BB6F89FD41FA}" id="{71D26F82-A9F5-4B83-AD60-E0722B6F3F61}" parentId="{67578144-E3EC-4152-8729-1B44EEC1002D}">
+    <text>And ms to s</text>
+  </threadedComment>
+  <threadedComment ref="F7" dT="2024-08-09T13:04:41.59" personId="{48458BD6-4CAC-498F-B01C-BB6F89FD41FA}" id="{6F7C1780-1EE0-4B0C-B03B-9322192D7EC2}">
+    <text>Log10 converted to normal -&gt; from scheme 3 table 1</text>
+  </threadedComment>
+  <threadedComment ref="F7" dT="2024-08-09T13:04:59.39" personId="{48458BD6-4CAC-498F-B01C-BB6F89FD41FA}" id="{DEF03100-DDD5-4206-85EB-F3BB046F00C3}" parentId="{6F7C1780-1EE0-4B0C-B03B-9322192D7EC2}">
+    <text>And ms to s</text>
+  </threadedComment>
   <threadedComment ref="B18" dT="2024-08-07T13:14:12.40" personId="{48458BD6-4CAC-498F-B01C-BB6F89FD41FA}" id="{B6F8C469-337C-40BE-B2DC-A13B6B68197A}">
     <text>Not modelled currently; we specify different off rates depending on whether camkii is P or not.</text>
   </threadedComment>
-  <threadedComment ref="N25" dT="2024-08-08T08:46:52.90" personId="{48458BD6-4CAC-498F-B01C-BB6F89FD41FA}" id="{6C2818CD-9DCB-407F-A713-A0F009955982}">
+  <threadedComment ref="P25" dT="2024-08-08T08:46:52.90" personId="{48458BD6-4CAC-498F-B01C-BB6F89FD41FA}" id="{6C2818CD-9DCB-407F-A713-A0F009955982}">
     <text>In this paper there is also k_mPP1 and k_onPP1 which should be checked to see how they are used</text>
   </threadedComment>
 </ThreadedComments>
@@ -1273,10 +1319,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B603CBE9-61C1-43B8-82FF-7D32E551985B}">
-  <dimension ref="A1:CU27"/>
+  <dimension ref="A1:CW27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,22 +1330,22 @@
     <col min="1" max="1" width="44.140625" style="4" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="9" width="11.7109375" customWidth="1"/>
-    <col min="10" max="11" width="11.7109375" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" customWidth="1"/>
-    <col min="13" max="15" width="14.5703125" customWidth="1"/>
-    <col min="16" max="16" width="25.28515625" customWidth="1"/>
-    <col min="17" max="17" width="13.42578125" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" customWidth="1"/>
-    <col min="19" max="19" width="11" customWidth="1"/>
-    <col min="20" max="29" width="12.5703125" customWidth="1"/>
+    <col min="4" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="11" width="11.7109375" customWidth="1"/>
+    <col min="12" max="13" width="11.7109375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="17" width="14.5703125" customWidth="1"/>
+    <col min="18" max="18" width="25.28515625" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" customWidth="1"/>
+    <col min="20" max="20" width="12.140625" customWidth="1"/>
+    <col min="21" max="21" width="11" customWidth="1"/>
+    <col min="22" max="31" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:101" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1316,13 +1362,13 @@
         <v>15</v>
       </c>
       <c r="F1" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="38" t="s">
         <v>20</v>
-      </c>
-      <c r="G1" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="38" t="s">
-        <v>15</v>
       </c>
       <c r="I1" s="38" t="s">
         <v>2</v>
@@ -1345,8 +1391,14 @@
       <c r="O1" s="38" t="s">
         <v>2</v>
       </c>
+      <c r="P1" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="38" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:99" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:101" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>40</v>
       </c>
@@ -1359,41 +1411,45 @@
       <c r="D2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="31">
+      <c r="E2" s="17">
+        <v>257000000</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="31">
         <v>25000000</v>
       </c>
-      <c r="F2" s="31">
+      <c r="H2" s="31">
         <v>260000000</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="I2" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="17">
+      <c r="J2" s="17">
         <v>770000000</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="K2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="26">
+      <c r="L2" s="26">
         <v>32200000000</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="M2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="35">
+      <c r="N2" s="35">
         <v>100000000</v>
       </c>
-      <c r="M2" s="36" t="s">
+      <c r="O2" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="26">
+      <c r="P2" s="26">
         <v>100000000</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="Q2" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="P2"/>
-      <c r="Q2"/>
       <c r="R2"/>
       <c r="S2"/>
       <c r="T2"/>
@@ -1476,8 +1532,10 @@
       <c r="CS2"/>
       <c r="CT2"/>
       <c r="CU2"/>
+      <c r="CV2"/>
+      <c r="CW2"/>
     </row>
-    <row r="3" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="6" t="s">
         <v>27</v>
@@ -1488,41 +1546,45 @@
       <c r="D3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="17">
+        <v>229000</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="31">
         <v>50000000</v>
       </c>
-      <c r="F3" s="31">
+      <c r="H3" s="31">
         <v>300000000</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="I3" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="17">
+      <c r="J3" s="17">
         <v>32000000000</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="K3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="26">
+      <c r="L3" s="26">
         <v>32200000000</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="M3" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="35">
+      <c r="N3" s="35">
         <v>150000000</v>
       </c>
-      <c r="M3" s="36" t="s">
+      <c r="O3" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="26">
+      <c r="P3" s="26">
         <v>150000000</v>
       </c>
-      <c r="O3" s="29" t="s">
+      <c r="Q3" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="P3"/>
-      <c r="Q3"/>
       <c r="R3"/>
       <c r="S3"/>
       <c r="T3"/>
@@ -1605,8 +1667,10 @@
       <c r="CS3"/>
       <c r="CT3"/>
       <c r="CU3"/>
+      <c r="CV3"/>
+      <c r="CW3"/>
     </row>
-    <row r="4" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="6" t="s">
         <v>24</v>
@@ -1617,41 +1681,45 @@
       <c r="D4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="17">
+        <v>21400000</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="31">
         <v>1200000</v>
       </c>
-      <c r="F4" s="31">
+      <c r="H4" s="31">
         <v>9600000</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="I4" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="17">
+      <c r="J4" s="17">
         <v>84000000</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="K4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="26">
+      <c r="L4" s="26">
         <v>322000000</v>
       </c>
-      <c r="K4" s="27" t="s">
+      <c r="M4" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="35">
+      <c r="N4" s="35">
         <v>4000000</v>
       </c>
-      <c r="M4" s="36" t="s">
+      <c r="O4" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="26">
+      <c r="P4" s="26">
         <v>4000000</v>
       </c>
-      <c r="O4" s="29" t="s">
+      <c r="Q4" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="P4"/>
-      <c r="Q4"/>
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
@@ -1734,8 +1802,10 @@
       <c r="CS4"/>
       <c r="CT4"/>
       <c r="CU4"/>
+      <c r="CV4"/>
+      <c r="CW4"/>
     </row>
-    <row r="5" spans="1:99" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:101" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="6" t="s">
         <v>25</v>
@@ -1746,41 +1816,45 @@
       <c r="D5" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="17">
+        <v>110000000</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="31">
         <v>5000000</v>
       </c>
-      <c r="F5" s="31">
+      <c r="H5" s="31">
         <v>25000000</v>
       </c>
-      <c r="G5" s="32" t="s">
+      <c r="I5" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="17">
+      <c r="J5" s="17">
         <v>250000000</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="K5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="26">
+      <c r="L5" s="26">
         <v>322000000</v>
       </c>
-      <c r="K5" s="27" t="s">
+      <c r="M5" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="35">
+      <c r="N5" s="35">
         <v>10000000</v>
       </c>
-      <c r="M5" s="36" t="s">
+      <c r="O5" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="26">
+      <c r="P5" s="26">
         <v>10000000</v>
       </c>
-      <c r="O5" s="29" t="s">
+      <c r="Q5" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="P5"/>
-      <c r="Q5"/>
       <c r="R5"/>
       <c r="S5"/>
       <c r="T5"/>
@@ -1863,8 +1937,10 @@
       <c r="CS5"/>
       <c r="CT5"/>
       <c r="CU5"/>
+      <c r="CV5"/>
+      <c r="CW5"/>
     </row>
-    <row r="6" spans="1:99" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:101" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>39</v>
       </c>
@@ -1880,26 +1956,24 @@
       <c r="E6" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="38"/>
+      <c r="G6" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="38" t="s">
         <v>20</v>
-      </c>
-      <c r="G6" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="38" t="s">
-        <v>23</v>
       </c>
       <c r="I6" s="38" t="s">
         <v>2</v>
       </c>
       <c r="J6" s="38" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="K6" s="38" t="s">
         <v>2</v>
       </c>
       <c r="L6" s="38" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="M6" s="38" t="s">
         <v>2</v>
@@ -1910,8 +1984,12 @@
       <c r="O6" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="P6"/>
-      <c r="Q6"/>
+      <c r="P6" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q6" s="38" t="s">
+        <v>2</v>
+      </c>
       <c r="R6"/>
       <c r="S6"/>
       <c r="T6"/>
@@ -1994,8 +2072,10 @@
       <c r="CS6"/>
       <c r="CT6"/>
       <c r="CU6"/>
+      <c r="CV6"/>
+      <c r="CW6"/>
     </row>
-    <row r="7" spans="1:99" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:101" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="6" t="s">
         <v>28</v>
@@ -2006,41 +2086,45 @@
       <c r="D7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="17">
+        <v>2040</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="31">
         <v>1000</v>
       </c>
-      <c r="F7" s="31">
+      <c r="H7" s="31">
         <v>4000</v>
       </c>
-      <c r="G7" s="32" t="s">
+      <c r="I7" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="17">
+      <c r="J7" s="17">
         <v>160000</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="K7" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="28">
+      <c r="L7" s="28">
         <v>9.3800000000000003E-5</v>
       </c>
-      <c r="K7" s="27" t="s">
+      <c r="M7" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="L7" s="35">
+      <c r="N7" s="35">
         <v>2660</v>
       </c>
-      <c r="M7" s="36" t="s">
+      <c r="O7" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="N7" s="26">
+      <c r="P7" s="26">
         <v>2660</v>
       </c>
-      <c r="O7" s="29" t="s">
+      <c r="Q7" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="P7"/>
-      <c r="Q7"/>
       <c r="R7"/>
       <c r="S7"/>
       <c r="T7"/>
@@ -2123,8 +2207,10 @@
       <c r="CS7"/>
       <c r="CT7"/>
       <c r="CU7"/>
+      <c r="CV7"/>
+      <c r="CW7"/>
     </row>
-    <row r="8" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="6" t="s">
         <v>29</v>
@@ -2135,41 +2221,45 @@
       <c r="D8" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="17">
+        <v>0.39</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="31">
         <v>500</v>
       </c>
-      <c r="F8" s="31">
+      <c r="H8" s="31">
         <v>1000</v>
       </c>
-      <c r="G8" s="32" t="s">
+      <c r="I8" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="17">
+      <c r="J8" s="17">
         <v>22000</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="K8" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="28">
+      <c r="L8" s="28">
         <v>9.3800000000000003E-5</v>
       </c>
-      <c r="K8" s="27" t="s">
+      <c r="M8" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="L8" s="35">
+      <c r="N8" s="35">
         <v>990</v>
       </c>
-      <c r="M8" s="36" t="s">
+      <c r="O8" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="26">
+      <c r="P8" s="26">
         <v>990</v>
       </c>
-      <c r="O8" s="29" t="s">
+      <c r="Q8" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="P8"/>
-      <c r="Q8"/>
       <c r="R8"/>
       <c r="S8"/>
       <c r="T8"/>
@@ -2252,8 +2342,10 @@
       <c r="CS8"/>
       <c r="CT8"/>
       <c r="CU8"/>
+      <c r="CV8"/>
+      <c r="CW8"/>
     </row>
-    <row r="9" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="6" t="s">
         <v>30</v>
@@ -2264,41 +2356,45 @@
       <c r="D9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="17">
+        <v>742</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="33">
         <v>10</v>
       </c>
-      <c r="F9" s="33">
+      <c r="H9" s="33">
         <v>70</v>
       </c>
-      <c r="G9" s="32" t="s">
+      <c r="I9" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="17">
+      <c r="J9" s="17">
         <v>2600</v>
       </c>
-      <c r="I9" s="18" t="s">
+      <c r="K9" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="28">
+      <c r="L9" s="28">
         <v>9.3800000000000003E-5</v>
       </c>
-      <c r="K9" s="27" t="s">
+      <c r="M9" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="37">
+      <c r="N9" s="37">
         <v>40.24</v>
       </c>
-      <c r="M9" s="36" t="s">
+      <c r="O9" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="30">
+      <c r="P9" s="30">
         <v>40.24</v>
       </c>
-      <c r="O9" s="29" t="s">
+      <c r="Q9" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="P9"/>
-      <c r="Q9"/>
       <c r="R9"/>
       <c r="S9"/>
       <c r="T9"/>
@@ -2381,8 +2477,10 @@
       <c r="CS9"/>
       <c r="CT9"/>
       <c r="CU9"/>
+      <c r="CV9"/>
+      <c r="CW9"/>
     </row>
-    <row r="10" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="6" t="s">
         <v>31</v>
@@ -2393,41 +2491,45 @@
       <c r="D10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="17">
+        <v>980</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="33">
         <v>8.5</v>
       </c>
-      <c r="F10" s="33">
+      <c r="H10" s="33">
         <v>10</v>
       </c>
-      <c r="G10" s="32" t="s">
+      <c r="I10" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="19">
+      <c r="J10" s="19">
         <v>6.5</v>
       </c>
-      <c r="I10" s="18" t="s">
+      <c r="K10" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="28">
+      <c r="L10" s="28">
         <v>9.3800000000000003E-5</v>
       </c>
-      <c r="K10" s="27" t="s">
+      <c r="M10" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="37">
+      <c r="N10" s="37">
         <v>9.3000000000000007</v>
       </c>
-      <c r="M10" s="36" t="s">
+      <c r="O10" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="N10" s="30">
+      <c r="P10" s="30">
         <v>9.3000000000000007</v>
       </c>
-      <c r="O10" s="29" t="s">
+      <c r="Q10" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="P10"/>
-      <c r="Q10"/>
       <c r="R10"/>
       <c r="S10"/>
       <c r="T10"/>
@@ -2510,8 +2612,10 @@
       <c r="CS10"/>
       <c r="CT10"/>
       <c r="CU10"/>
+      <c r="CV10"/>
+      <c r="CW10"/>
     </row>
-    <row r="11" spans="1:99" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:101" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>3</v>
       </c>
@@ -2524,14 +2628,16 @@
       <c r="D11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="1"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="L11" s="1"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="1:99" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:101" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="7" t="s">
         <v>5</v>
@@ -2542,14 +2648,16 @@
       <c r="D12" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="L12" s="1"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="1:99" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:101" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="38" t="s">
         <v>14</v>
@@ -2560,17 +2668,13 @@
       <c r="D13" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="38" t="s">
+      <c r="H13" s="38" t="s">
         <v>20</v>
-      </c>
-      <c r="G13" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="38" t="s">
-        <v>15</v>
       </c>
       <c r="I13" s="38" t="s">
         <v>2</v>
@@ -2593,8 +2697,14 @@
       <c r="O13" s="38" t="s">
         <v>2</v>
       </c>
+      <c r="P13" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q13" s="38" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="14" spans="1:99" s="2" customFormat="1" ht="33.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:101" s="2" customFormat="1" ht="33.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>42</v>
       </c>
@@ -2607,32 +2717,28 @@
       <c r="D14" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="31">
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="31">
         <v>1400000</v>
       </c>
-      <c r="F14" s="31">
+      <c r="H14" s="31">
         <v>60000000</v>
       </c>
-      <c r="G14" s="32" t="s">
+      <c r="I14" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="J14" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="K14" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="J14" s="10">
+      <c r="L14" s="10">
         <v>2860000</v>
       </c>
-      <c r="K14" s="8" t="s">
+      <c r="M14" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="L14" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="M14" s="14" t="s">
-        <v>35</v>
       </c>
       <c r="N14" s="14" t="s">
         <v>35</v>
@@ -2640,8 +2746,12 @@
       <c r="O14" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="P14"/>
-      <c r="Q14"/>
+      <c r="P14" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q14" s="14" t="s">
+        <v>35</v>
+      </c>
       <c r="R14"/>
       <c r="S14"/>
       <c r="T14"/>
@@ -2724,8 +2834,10 @@
       <c r="CS14"/>
       <c r="CT14"/>
       <c r="CU14"/>
+      <c r="CV14"/>
+      <c r="CW14"/>
     </row>
-    <row r="15" spans="1:99" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="6" t="s">
         <v>36</v>
@@ -2736,43 +2848,43 @@
       <c r="D15" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="31" t="s">
+      <c r="H15" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="32" t="s">
+      <c r="I15" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="J15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="K15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="10" t="s">
+      <c r="L15" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K15" s="8" t="s">
+      <c r="M15" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="L15" s="35">
+      <c r="N15" s="35">
         <v>30000000</v>
       </c>
-      <c r="M15" s="36" t="s">
+      <c r="O15" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="N15" s="26">
+      <c r="P15" s="26">
         <v>30000000</v>
       </c>
-      <c r="O15" s="29" t="s">
+      <c r="Q15" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="P15"/>
-      <c r="Q15" s="15"/>
       <c r="R15"/>
-      <c r="S15"/>
+      <c r="S15" s="15"/>
       <c r="T15"/>
       <c r="U15"/>
       <c r="V15"/>
@@ -2853,8 +2965,10 @@
       <c r="CS15"/>
       <c r="CT15"/>
       <c r="CU15"/>
+      <c r="CV15"/>
+      <c r="CW15"/>
     </row>
-    <row r="16" spans="1:99" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:101" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12"/>
       <c r="B16" s="6" t="s">
         <v>37</v>
@@ -2865,43 +2979,43 @@
       <c r="D16" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="H16" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="32" t="s">
+      <c r="I16" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="J16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="K16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="L16" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="M16" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="L16" s="35">
+      <c r="N16" s="35">
         <v>10000000</v>
       </c>
-      <c r="M16" s="36" t="s">
+      <c r="O16" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="N16" s="26">
+      <c r="P16" s="26">
         <v>50000000</v>
       </c>
-      <c r="O16" s="29" t="s">
+      <c r="Q16" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="P16"/>
-      <c r="Q16" s="15"/>
       <c r="R16"/>
-      <c r="S16"/>
+      <c r="S16" s="15"/>
       <c r="T16"/>
       <c r="U16"/>
       <c r="V16"/>
@@ -2982,8 +3096,10 @@
       <c r="CS16"/>
       <c r="CT16"/>
       <c r="CU16"/>
+      <c r="CV16"/>
+      <c r="CW16"/>
     </row>
-    <row r="17" spans="1:99" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:101" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
       <c r="B17" s="38" t="s">
         <v>1</v>
@@ -2994,29 +3110,25 @@
       <c r="D17" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="38" t="s">
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="38" t="s">
+      <c r="H17" s="38" t="s">
         <v>20</v>
-      </c>
-      <c r="G17" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="H17" s="38" t="s">
-        <v>23</v>
       </c>
       <c r="I17" s="38" t="s">
         <v>2</v>
       </c>
       <c r="J17" s="38" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="K17" s="38" t="s">
         <v>2</v>
       </c>
       <c r="L17" s="38" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="M17" s="38" t="s">
         <v>2</v>
@@ -3027,10 +3139,14 @@
       <c r="O17" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="P17"/>
-      <c r="Q17" s="15"/>
+      <c r="P17" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q17" s="38" t="s">
+        <v>2</v>
+      </c>
       <c r="R17"/>
-      <c r="S17"/>
+      <c r="S17" s="15"/>
       <c r="T17"/>
       <c r="U17"/>
       <c r="V17"/>
@@ -3111,8 +3227,10 @@
       <c r="CS17"/>
       <c r="CT17"/>
       <c r="CU17"/>
+      <c r="CV17"/>
+      <c r="CW17"/>
     </row>
-    <row r="18" spans="1:99" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:101" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>41</v>
       </c>
@@ -3125,41 +3243,43 @@
       <c r="D18" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="33">
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="33">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F18" s="33">
+      <c r="H18" s="33">
         <v>2.2999999999999998</v>
       </c>
-      <c r="G18" s="32" t="s">
+      <c r="I18" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="J18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="K18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J18" s="9">
+      <c r="L18" s="9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K18" s="8" t="s">
+      <c r="M18" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L18" s="37" t="s">
+      <c r="N18" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="M18" s="37" t="s">
+      <c r="O18" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="N18" s="30" t="s">
+      <c r="P18" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="O18" s="29" t="s">
+      <c r="Q18" s="29" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="7" t="s">
         <v>7</v>
@@ -3170,41 +3290,43 @@
       <c r="D19" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="33" t="s">
+      <c r="H19" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="32" t="s">
+      <c r="I19" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="J19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="K19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J19" s="9" t="s">
+      <c r="L19" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="M19" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="L19" s="37">
+      <c r="N19" s="37">
         <v>1.95</v>
       </c>
-      <c r="M19" s="36" t="s">
+      <c r="O19" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="N19" s="30">
+      <c r="P19" s="30">
         <v>1.95</v>
       </c>
-      <c r="O19" s="29" t="s">
+      <c r="Q19" s="29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:99" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:101" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
       <c r="B20" s="7" t="s">
         <v>8</v>
@@ -3215,41 +3337,43 @@
       <c r="D20" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="33" t="s">
+      <c r="H20" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="32" t="s">
+      <c r="I20" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="J20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="K20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J20" s="9" t="s">
+      <c r="L20" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="K20" s="8" t="s">
+      <c r="M20" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="L20" s="37">
+      <c r="N20" s="37">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M20" s="36" t="s">
+      <c r="O20" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="N20" s="26">
+      <c r="P20" s="26">
         <v>9.0000000000000006E-5</v>
       </c>
-      <c r="O20" s="29" t="s">
+      <c r="Q20" s="29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:99" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:101" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11"/>
       <c r="B21" s="38" t="s">
         <v>14</v>
@@ -3260,29 +3384,25 @@
       <c r="D21" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="38" t="s">
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="38" t="s">
+      <c r="H21" s="38" t="s">
         <v>20</v>
-      </c>
-      <c r="G21" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="H21" s="38" t="s">
-        <v>23</v>
       </c>
       <c r="I21" s="38" t="s">
         <v>2</v>
       </c>
       <c r="J21" s="38" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="K21" s="38" t="s">
         <v>2</v>
       </c>
       <c r="L21" s="38" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="M21" s="38" t="s">
         <v>2</v>
@@ -3293,8 +3413,14 @@
       <c r="O21" s="38" t="s">
         <v>2</v>
       </c>
+      <c r="P21" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q21" s="38" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="22" spans="1:99" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:101" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>9</v>
       </c>
@@ -3307,36 +3433,36 @@
       <c r="D22" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="33">
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="33">
         <v>0.5</v>
       </c>
-      <c r="F22" s="33">
+      <c r="H22" s="33">
         <v>1.25</v>
       </c>
-      <c r="G22" s="32" t="s">
+      <c r="I22" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="J22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="K22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J22" s="3"/>
-      <c r="L22" s="37">
+      <c r="L22" s="3"/>
+      <c r="N22" s="37">
         <v>0.96</v>
       </c>
-      <c r="M22" s="36" t="s">
+      <c r="O22" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="N22" s="30">
+      <c r="P22" s="30">
         <v>0.96</v>
       </c>
-      <c r="O22" s="29" t="s">
+      <c r="Q22" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="P22"/>
-      <c r="Q22"/>
       <c r="R22"/>
       <c r="S22"/>
       <c r="T22"/>
@@ -3387,8 +3513,10 @@
       <c r="BM22"/>
       <c r="BN22"/>
       <c r="BO22"/>
+      <c r="BP22"/>
+      <c r="BQ22"/>
     </row>
-    <row r="23" spans="1:99" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:101" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>10</v>
       </c>
@@ -3401,35 +3529,37 @@
       <c r="D23" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="46">
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="46">
         <v>0.01</v>
       </c>
-      <c r="F23" s="44">
+      <c r="H23" s="44">
         <v>0.05</v>
       </c>
-      <c r="G23" s="45" t="s">
+      <c r="I23" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="H23" s="42" t="s">
+      <c r="J23" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="I23" s="43" t="s">
+      <c r="K23" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="L23" s="37" t="s">
+      <c r="N23" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="M23" s="37" t="s">
+      <c r="O23" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="N23" s="30" t="s">
+      <c r="P23" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="O23" s="30" t="s">
+      <c r="Q23" s="30" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:99" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:101" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
       <c r="B24" s="38" t="s">
         <v>1</v>
@@ -3440,29 +3570,25 @@
       <c r="D24" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E24" s="38" t="s">
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="38" t="s">
+      <c r="H24" s="38" t="s">
         <v>20</v>
-      </c>
-      <c r="G24" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="H24" s="38" t="s">
-        <v>23</v>
       </c>
       <c r="I24" s="38" t="s">
         <v>2</v>
       </c>
       <c r="J24" s="38" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="K24" s="38" t="s">
         <v>2</v>
       </c>
       <c r="L24" s="38" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="M24" s="38" t="s">
         <v>2</v>
@@ -3470,11 +3596,17 @@
       <c r="N24" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="O24" s="16" t="s">
+      <c r="O24" s="38" t="s">
         <v>2</v>
       </c>
+      <c r="P24" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q24" s="16" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="25" spans="1:99" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:101" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>11</v>
       </c>
@@ -3487,24 +3619,24 @@
       <c r="D25" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="34"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="40"/>
       <c r="J25" s="3"/>
-      <c r="L25" s="33">
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="N25" s="33">
         <v>0.41</v>
       </c>
-      <c r="M25" s="36" t="s">
+      <c r="O25" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="N25" s="25">
+      <c r="P25" s="25">
         <v>11.5</v>
       </c>
-      <c r="O25" s="25"/>
-      <c r="P25"/>
-      <c r="Q25"/>
+      <c r="Q25" s="25"/>
       <c r="R25"/>
       <c r="S25"/>
       <c r="T25"/>
@@ -3555,13 +3687,15 @@
       <c r="BM25"/>
       <c r="BN25"/>
       <c r="BO25"/>
+      <c r="BP25"/>
+      <c r="BQ25"/>
     </row>
-    <row r="26" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
domas rxn rates added to model
</commit_message>
<xml_diff>
--- a/rxns_table.xlsx
+++ b/rxns_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD_2023\CaMKII_hexa_bgnl_to_mcell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B674CA7-6D22-4BCB-A652-53AEDFE8C568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1258EC2-031D-473F-9675-79C43B93E5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4B4FB280-5B08-406D-B059-D87F72317E26}"/>
   </bookViews>
@@ -1322,7 +1322,7 @@
   <dimension ref="A1:CW27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
domas' parameters plus observables fixed
</commit_message>
<xml_diff>
--- a/rxns_table.xlsx
+++ b/rxns_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD_2023\CaMKII_hexa_bgnl_to_mcell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1258EC2-031D-473F-9675-79C43B93E5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5560F22F-B488-4AEE-880F-F8E62D44D3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4B4FB280-5B08-406D-B059-D87F72317E26}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="56">
   <si>
     <t>Description</t>
   </si>
@@ -272,6 +272,9 @@
   </si>
   <si>
     <t>Linkevicius et al., 2027</t>
+  </si>
+  <si>
+    <t>Meyer et al., 1992</t>
   </si>
 </sst>
 </file>
@@ -467,7 +470,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -686,6 +689,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -850,7 +859,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -881,8 +890,6 @@
     <xf numFmtId="0" fontId="21" fillId="36" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="36" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="36" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="21" fillId="36" borderId="0" xfId="6" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="18" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="21" fillId="36" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -908,6 +915,12 @@
     <xf numFmtId="0" fontId="21" fillId="39" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="18" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="22" fillId="33" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="21" fillId="33" borderId="0" xfId="6" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="21" fillId="40" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="22" fillId="40" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="40" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1322,7 +1335,7 @@
   <dimension ref="A1:CW27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,52 +1362,52 @@
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="38" t="s">
+      <c r="D1" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="38" t="s">
+      <c r="F1" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="38" t="s">
+      <c r="I1" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="38" t="s">
+      <c r="K1" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="38" t="s">
+      <c r="M1" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" s="38" t="s">
+      <c r="O1" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="38" t="s">
+      <c r="Q1" s="36" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1417,13 +1430,13 @@
       <c r="F2" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="31">
+      <c r="G2" s="29">
         <v>25000000</v>
       </c>
-      <c r="H2" s="31">
+      <c r="H2" s="29">
         <v>260000000</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="30" t="s">
         <v>19</v>
       </c>
       <c r="J2" s="17">
@@ -1432,22 +1445,22 @@
       <c r="K2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="26">
+      <c r="L2" s="24">
         <v>32200000000</v>
       </c>
-      <c r="M2" s="27" t="s">
+      <c r="M2" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="35">
+      <c r="N2" s="33">
         <v>100000000</v>
       </c>
-      <c r="O2" s="36" t="s">
+      <c r="O2" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="26">
+      <c r="P2" s="24">
         <v>100000000</v>
       </c>
-      <c r="Q2" s="29" t="s">
+      <c r="Q2" s="27" t="s">
         <v>22</v>
       </c>
       <c r="R2"/>
@@ -1552,13 +1565,13 @@
       <c r="F3" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="31">
+      <c r="G3" s="29">
         <v>50000000</v>
       </c>
-      <c r="H3" s="31">
+      <c r="H3" s="29">
         <v>300000000</v>
       </c>
-      <c r="I3" s="32" t="s">
+      <c r="I3" s="30" t="s">
         <v>19</v>
       </c>
       <c r="J3" s="17">
@@ -1567,22 +1580,22 @@
       <c r="K3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="26">
+      <c r="L3" s="24">
         <v>32200000000</v>
       </c>
-      <c r="M3" s="27" t="s">
+      <c r="M3" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="N3" s="35">
+      <c r="N3" s="33">
         <v>150000000</v>
       </c>
-      <c r="O3" s="36" t="s">
+      <c r="O3" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="26">
+      <c r="P3" s="24">
         <v>150000000</v>
       </c>
-      <c r="Q3" s="29" t="s">
+      <c r="Q3" s="27" t="s">
         <v>22</v>
       </c>
       <c r="R3"/>
@@ -1687,13 +1700,13 @@
       <c r="F4" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="29">
         <v>1200000</v>
       </c>
-      <c r="H4" s="31">
+      <c r="H4" s="29">
         <v>9600000</v>
       </c>
-      <c r="I4" s="32" t="s">
+      <c r="I4" s="30" t="s">
         <v>19</v>
       </c>
       <c r="J4" s="17">
@@ -1702,22 +1715,22 @@
       <c r="K4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="26">
+      <c r="L4" s="24">
         <v>322000000</v>
       </c>
-      <c r="M4" s="27" t="s">
+      <c r="M4" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="35">
+      <c r="N4" s="33">
         <v>4000000</v>
       </c>
-      <c r="O4" s="36" t="s">
+      <c r="O4" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="26">
+      <c r="P4" s="24">
         <v>4000000</v>
       </c>
-      <c r="Q4" s="29" t="s">
+      <c r="Q4" s="27" t="s">
         <v>22</v>
       </c>
       <c r="R4"/>
@@ -1822,13 +1835,13 @@
       <c r="F5" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="29">
         <v>5000000</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="29">
         <v>25000000</v>
       </c>
-      <c r="I5" s="32" t="s">
+      <c r="I5" s="30" t="s">
         <v>19</v>
       </c>
       <c r="J5" s="17">
@@ -1837,22 +1850,22 @@
       <c r="K5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="26">
+      <c r="L5" s="24">
         <v>322000000</v>
       </c>
-      <c r="M5" s="27" t="s">
+      <c r="M5" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="35">
+      <c r="N5" s="33">
         <v>10000000</v>
       </c>
-      <c r="O5" s="36" t="s">
+      <c r="O5" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="P5" s="26">
+      <c r="P5" s="24">
         <v>10000000</v>
       </c>
-      <c r="Q5" s="29" t="s">
+      <c r="Q5" s="27" t="s">
         <v>22</v>
       </c>
       <c r="R5"/>
@@ -1944,50 +1957,50 @@
       <c r="A6" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="38" t="s">
+      <c r="D6" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38" t="s">
+      <c r="F6" s="36"/>
+      <c r="G6" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="38" t="s">
+      <c r="H6" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="38" t="s">
+      <c r="I6" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="L6" s="38" t="s">
+      <c r="K6" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="N6" s="38" t="s">
+      <c r="M6" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="N6" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="O6" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="P6" s="38" t="s">
+      <c r="O6" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="Q6" s="38" t="s">
+      <c r="Q6" s="36" t="s">
         <v>2</v>
       </c>
       <c r="R6"/>
@@ -2092,13 +2105,13 @@
       <c r="F7" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="31">
+      <c r="G7" s="29">
         <v>1000</v>
       </c>
-      <c r="H7" s="31">
+      <c r="H7" s="29">
         <v>4000</v>
       </c>
-      <c r="I7" s="32" t="s">
+      <c r="I7" s="30" t="s">
         <v>19</v>
       </c>
       <c r="J7" s="17">
@@ -2107,22 +2120,22 @@
       <c r="K7" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="28">
+      <c r="L7" s="26">
         <v>9.3800000000000003E-5</v>
       </c>
-      <c r="M7" s="27" t="s">
+      <c r="M7" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="N7" s="35">
+      <c r="N7" s="33">
         <v>2660</v>
       </c>
-      <c r="O7" s="36" t="s">
+      <c r="O7" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="P7" s="26">
+      <c r="P7" s="24">
         <v>2660</v>
       </c>
-      <c r="Q7" s="29" t="s">
+      <c r="Q7" s="27" t="s">
         <v>22</v>
       </c>
       <c r="R7"/>
@@ -2227,13 +2240,13 @@
       <c r="F8" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="31">
+      <c r="G8" s="29">
         <v>500</v>
       </c>
-      <c r="H8" s="31">
+      <c r="H8" s="29">
         <v>1000</v>
       </c>
-      <c r="I8" s="32" t="s">
+      <c r="I8" s="30" t="s">
         <v>19</v>
       </c>
       <c r="J8" s="17">
@@ -2242,22 +2255,22 @@
       <c r="K8" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="28">
+      <c r="L8" s="26">
         <v>9.3800000000000003E-5</v>
       </c>
-      <c r="M8" s="27" t="s">
+      <c r="M8" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="N8" s="35">
+      <c r="N8" s="33">
         <v>990</v>
       </c>
-      <c r="O8" s="36" t="s">
+      <c r="O8" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="P8" s="26">
+      <c r="P8" s="24">
         <v>990</v>
       </c>
-      <c r="Q8" s="29" t="s">
+      <c r="Q8" s="27" t="s">
         <v>22</v>
       </c>
       <c r="R8"/>
@@ -2362,13 +2375,13 @@
       <c r="F9" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="33">
+      <c r="G9" s="31">
         <v>10</v>
       </c>
-      <c r="H9" s="33">
+      <c r="H9" s="31">
         <v>70</v>
       </c>
-      <c r="I9" s="32" t="s">
+      <c r="I9" s="30" t="s">
         <v>19</v>
       </c>
       <c r="J9" s="17">
@@ -2377,22 +2390,22 @@
       <c r="K9" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="L9" s="28">
+      <c r="L9" s="26">
         <v>9.3800000000000003E-5</v>
       </c>
-      <c r="M9" s="27" t="s">
+      <c r="M9" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="N9" s="37">
+      <c r="N9" s="35">
         <v>40.24</v>
       </c>
-      <c r="O9" s="36" t="s">
+      <c r="O9" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="30">
+      <c r="P9" s="28">
         <v>40.24</v>
       </c>
-      <c r="Q9" s="29" t="s">
+      <c r="Q9" s="27" t="s">
         <v>22</v>
       </c>
       <c r="R9"/>
@@ -2497,13 +2510,13 @@
       <c r="F10" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="33">
+      <c r="G10" s="31">
         <v>8.5</v>
       </c>
-      <c r="H10" s="33">
+      <c r="H10" s="31">
         <v>10</v>
       </c>
-      <c r="I10" s="32" t="s">
+      <c r="I10" s="30" t="s">
         <v>19</v>
       </c>
       <c r="J10" s="19">
@@ -2512,22 +2525,22 @@
       <c r="K10" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="L10" s="28">
+      <c r="L10" s="26">
         <v>9.3800000000000003E-5</v>
       </c>
-      <c r="M10" s="27" t="s">
+      <c r="M10" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="N10" s="37">
+      <c r="N10" s="35">
         <v>9.3000000000000007</v>
       </c>
-      <c r="O10" s="36" t="s">
+      <c r="O10" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="P10" s="30">
+      <c r="P10" s="28">
         <v>9.3000000000000007</v>
       </c>
-      <c r="Q10" s="29" t="s">
+      <c r="Q10" s="27" t="s">
         <v>22</v>
       </c>
       <c r="R10"/>
@@ -2659,48 +2672,52 @@
     </row>
     <row r="13" spans="1:101" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38" t="s">
+      <c r="D13" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="38" t="s">
+      <c r="F13" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" s="38" t="s">
+      <c r="I13" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="L13" s="38" t="s">
+      <c r="K13" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="L13" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="M13" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="N13" s="38" t="s">
+      <c r="M13" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="N13" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="O13" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="P13" s="38" t="s">
+      <c r="O13" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="P13" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="Q13" s="38" t="s">
+      <c r="Q13" s="36" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2717,15 +2734,19 @@
       <c r="D14" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="31">
+      <c r="E14" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="29">
         <v>1400000</v>
       </c>
-      <c r="H14" s="31">
+      <c r="H14" s="29">
         <v>60000000</v>
       </c>
-      <c r="I14" s="32" t="s">
+      <c r="I14" s="30" t="s">
         <v>19</v>
       </c>
       <c r="J14" s="14" t="s">
@@ -2842,21 +2863,25 @@
       <c r="B15" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="31" t="s">
+      <c r="E15" s="48">
+        <v>150000000</v>
+      </c>
+      <c r="F15" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="31" t="s">
+      <c r="H15" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="I15" s="32" t="s">
+      <c r="I15" s="30" t="s">
         <v>35</v>
       </c>
       <c r="J15" s="3" t="s">
@@ -2871,16 +2896,16 @@
       <c r="M15" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="N15" s="35">
+      <c r="N15" s="33">
         <v>30000000</v>
       </c>
-      <c r="O15" s="36" t="s">
+      <c r="O15" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="P15" s="26">
+      <c r="P15" s="24">
         <v>30000000</v>
       </c>
-      <c r="Q15" s="29" t="s">
+      <c r="Q15" s="27" t="s">
         <v>22</v>
       </c>
       <c r="R15"/>
@@ -2973,21 +2998,25 @@
       <c r="B16" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="31" t="s">
+      <c r="E16" s="48">
+        <v>50000000</v>
+      </c>
+      <c r="F16" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="H16" s="31" t="s">
+      <c r="H16" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="I16" s="32" t="s">
+      <c r="I16" s="30" t="s">
         <v>35</v>
       </c>
       <c r="J16" s="3" t="s">
@@ -3002,16 +3031,16 @@
       <c r="M16" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="N16" s="35">
+      <c r="N16" s="33">
         <v>10000000</v>
       </c>
-      <c r="O16" s="36" t="s">
+      <c r="O16" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="P16" s="26">
+      <c r="P16" s="24">
         <v>50000000</v>
       </c>
-      <c r="Q16" s="29" t="s">
+      <c r="Q16" s="27" t="s">
         <v>22</v>
       </c>
       <c r="R16"/>
@@ -3101,48 +3130,52 @@
     </row>
     <row r="17" spans="1:101" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="38" t="s">
+      <c r="C17" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38" t="s">
+      <c r="D17" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="H17" s="38" t="s">
+      <c r="F17" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="I17" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="J17" s="38" t="s">
+      <c r="I17" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="L17" s="38" t="s">
+      <c r="K17" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="L17" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="M17" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="N17" s="38" t="s">
+      <c r="M17" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="N17" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="O17" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="P17" s="38" t="s">
+      <c r="O17" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="P17" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="Q17" s="38" t="s">
+      <c r="Q17" s="36" t="s">
         <v>2</v>
       </c>
       <c r="R17"/>
@@ -3243,15 +3276,19 @@
       <c r="D18" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="33">
+      <c r="E18" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="31">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H18" s="33">
+      <c r="H18" s="31">
         <v>2.2999999999999998</v>
       </c>
-      <c r="I18" s="32" t="s">
+      <c r="I18" s="30" t="s">
         <v>19</v>
       </c>
       <c r="J18" s="2" t="s">
@@ -3266,16 +3303,16 @@
       <c r="M18" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="N18" s="37" t="s">
+      <c r="N18" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="O18" s="37" t="s">
+      <c r="O18" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="P18" s="30" t="s">
+      <c r="P18" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="Q18" s="29" t="s">
+      <c r="Q18" s="27" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3284,21 +3321,25 @@
       <c r="B19" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="33" t="s">
+      <c r="E19" s="50">
+        <v>0.46</v>
+      </c>
+      <c r="F19" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="H19" s="33" t="s">
+      <c r="H19" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="I19" s="32" t="s">
+      <c r="I19" s="30" t="s">
         <v>34</v>
       </c>
       <c r="J19" s="2" t="s">
@@ -3313,16 +3354,16 @@
       <c r="M19" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="N19" s="37">
+      <c r="N19" s="35">
         <v>1.95</v>
       </c>
-      <c r="O19" s="36" t="s">
+      <c r="O19" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="P19" s="30">
+      <c r="P19" s="28">
         <v>1.95</v>
       </c>
-      <c r="Q19" s="29" t="s">
+      <c r="Q19" s="27" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3331,21 +3372,25 @@
       <c r="B20" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="33" t="s">
+      <c r="E20" s="48">
+        <v>1000</v>
+      </c>
+      <c r="F20" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="H20" s="33" t="s">
+      <c r="H20" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="I20" s="32" t="s">
+      <c r="I20" s="30" t="s">
         <v>34</v>
       </c>
       <c r="J20" s="2" t="s">
@@ -3360,63 +3405,63 @@
       <c r="M20" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="N20" s="37">
+      <c r="N20" s="35">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="O20" s="36" t="s">
+      <c r="O20" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="P20" s="26">
+      <c r="P20" s="24">
         <v>9.0000000000000006E-5</v>
       </c>
-      <c r="Q20" s="29" t="s">
+      <c r="Q20" s="27" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:101" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11"/>
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38" t="s">
+      <c r="D21" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="H21" s="38" t="s">
+      <c r="H21" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="I21" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="J21" s="38" t="s">
+      <c r="I21" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="J21" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="K21" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="L21" s="38" t="s">
+      <c r="K21" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="L21" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="M21" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="N21" s="38" t="s">
+      <c r="M21" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="N21" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="O21" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="P21" s="38" t="s">
+      <c r="O21" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="P21" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="Q21" s="38" t="s">
+      <c r="Q21" s="36" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3427,21 +3472,21 @@
       <c r="B22" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="25">
+      <c r="C22" s="23">
         <v>10</v>
       </c>
-      <c r="D22" s="24" t="s">
+      <c r="D22" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="33">
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="31">
         <v>0.5</v>
       </c>
-      <c r="H22" s="33">
+      <c r="H22" s="31">
         <v>1.25</v>
       </c>
-      <c r="I22" s="32" t="s">
+      <c r="I22" s="30" t="s">
         <v>19</v>
       </c>
       <c r="J22" s="2" t="s">
@@ -3451,16 +3496,16 @@
         <v>34</v>
       </c>
       <c r="L22" s="3"/>
-      <c r="N22" s="37">
+      <c r="N22" s="35">
         <v>0.96</v>
       </c>
-      <c r="O22" s="36" t="s">
+      <c r="O22" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="P22" s="30">
+      <c r="P22" s="28">
         <v>0.96</v>
       </c>
-      <c r="Q22" s="29" t="s">
+      <c r="Q22" s="27" t="s">
         <v>22</v>
       </c>
       <c r="R22"/>
@@ -3523,83 +3568,83 @@
       <c r="B23" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="41">
+      <c r="C23" s="39">
         <v>0.02</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="D23" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="46">
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="44">
         <v>0.01</v>
       </c>
-      <c r="H23" s="44">
+      <c r="H23" s="42">
         <v>0.05</v>
       </c>
-      <c r="I23" s="45" t="s">
+      <c r="I23" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="J23" s="42" t="s">
+      <c r="J23" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="K23" s="43" t="s">
+      <c r="K23" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="N23" s="37" t="s">
+      <c r="N23" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="O23" s="37" t="s">
+      <c r="O23" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="P23" s="30" t="s">
+      <c r="P23" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="Q23" s="30" t="s">
+      <c r="Q23" s="28" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:101" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="38" t="s">
+      <c r="C24" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38" t="s">
+      <c r="D24" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="H24" s="38" t="s">
+      <c r="H24" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="I24" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="J24" s="38" t="s">
+      <c r="I24" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="J24" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="K24" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="L24" s="38" t="s">
+      <c r="K24" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="L24" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="M24" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="N24" s="38" t="s">
+      <c r="M24" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="N24" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="O24" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="P24" s="38" t="s">
+      <c r="O24" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="P24" s="36" t="s">
         <v>23</v>
       </c>
       <c r="Q24" s="16" t="s">
@@ -3613,30 +3658,30 @@
       <c r="B25" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="39">
+      <c r="C25" s="37">
         <v>20</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="D25" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="40"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="38"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
-      <c r="N25" s="33">
+      <c r="N25" s="31">
         <v>0.41</v>
       </c>
-      <c r="O25" s="36" t="s">
+      <c r="O25" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="P25" s="25">
+      <c r="P25" s="23">
         <v>11.5</v>
       </c>
-      <c r="Q25" s="25"/>
+      <c r="Q25" s="23"/>
       <c r="R25"/>
       <c r="S25"/>
       <c r="T25"/>

</xml_diff>

<commit_message>
some files will need to be deleted; commiting to keep track of changes but probs files run pre 20240905 are not saved correctly due to overwriting of params
</commit_message>
<xml_diff>
--- a/rxns_table.xlsx
+++ b/rxns_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD_2023\CaMKII_hexa_bgnl_to_mcell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5560F22F-B488-4AEE-880F-F8E62D44D3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A618A38-8E02-40BE-856D-6A386AE4F1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4B4FB280-5B08-406D-B059-D87F72317E26}"/>
   </bookViews>
@@ -37,6 +37,7 @@
   <authors>
     <author>tc={67578144-E3EC-4152-8729-1B44EEC1002D}</author>
     <author>tc={6F7C1780-1EE0-4B0C-B03B-9322192D7EC2}</author>
+    <author>tc={802EEB37-19A7-4071-9209-8ED3C607D4E8}</author>
     <author>tc={B6F8C469-337C-40BE-B2DC-A13B6B68197A}</author>
     <author>Susana Roman</author>
     <author>tc={6C2818CD-9DCB-407F-A713-A0F009955982}</author>
@@ -62,7 +63,16 @@
     And ms to s</t>
       </text>
     </comment>
-    <comment ref="B18" authorId="2" shapeId="0" xr:uid="{B6F8C469-337C-40BE-B2DC-A13B6B68197A}">
+    <comment ref="J14" authorId="2" shapeId="0" xr:uid="{802EEB37-19A7-4071-9209-8ED3C607D4E8}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Range 1.6 and 3.4×106 Mol−1
+</t>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="3" shapeId="0" xr:uid="{B6F8C469-337C-40BE-B2DC-A13B6B68197A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -70,7 +80,31 @@
     Not modelled currently; we specify different off rates depending on whether camkii is P or not.</t>
       </text>
     </comment>
-    <comment ref="N22" authorId="3" shapeId="0" xr:uid="{D783E934-AE8E-45F6-BF32-CFA5F3DEAB20}">
+    <comment ref="P19" authorId="4" shapeId="0" xr:uid="{7C16AAE1-EC76-4DE7-BC28-A2AA54E7931D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Susana Roman:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+need to x check these as surely unbinding from phosphorylated camkii is slower/less likely than unbinding from unP?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N22" authorId="4" shapeId="0" xr:uid="{D783E934-AE8E-45F6-BF32-CFA5F3DEAB20}">
       <text>
         <r>
           <rPr>
@@ -94,7 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P25" authorId="4" shapeId="0" xr:uid="{6C2818CD-9DCB-407F-A713-A0F009955982}">
+    <comment ref="P25" authorId="5" shapeId="0" xr:uid="{6C2818CD-9DCB-407F-A713-A0F009955982}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -107,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="57">
   <si>
     <t>Description</t>
   </si>
@@ -275,6 +309,9 @@
   </si>
   <si>
     <t>Meyer et al., 1992</t>
+  </si>
+  <si>
+    <t>Rellos et al., 2010</t>
   </si>
 </sst>
 </file>
@@ -859,7 +896,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -921,6 +958,8 @@
     <xf numFmtId="11" fontId="21" fillId="40" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="22" fillId="40" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="40" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="21" fillId="38" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1321,6 +1360,10 @@
   <threadedComment ref="F7" dT="2024-08-09T13:04:59.39" personId="{48458BD6-4CAC-498F-B01C-BB6F89FD41FA}" id="{DEF03100-DDD5-4206-85EB-F3BB046F00C3}" parentId="{6F7C1780-1EE0-4B0C-B03B-9322192D7EC2}">
     <text>And ms to s</text>
   </threadedComment>
+  <threadedComment ref="J14" dT="2024-08-21T16:42:04.13" personId="{48458BD6-4CAC-498F-B01C-BB6F89FD41FA}" id="{802EEB37-19A7-4071-9209-8ED3C607D4E8}">
+    <text xml:space="preserve">Range 1.6 and 3.4×106 Mol−1
+</text>
+  </threadedComment>
   <threadedComment ref="B18" dT="2024-08-07T13:14:12.40" personId="{48458BD6-4CAC-498F-B01C-BB6F89FD41FA}" id="{B6F8C469-337C-40BE-B2DC-A13B6B68197A}">
     <text>Not modelled currently; we specify different off rates depending on whether camkii is P or not.</text>
   </threadedComment>
@@ -1335,7 +1378,7 @@
   <dimension ref="A1:CW27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2749,11 +2792,11 @@
       <c r="I14" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="K14" s="14" t="s">
-        <v>35</v>
+      <c r="J14" s="51">
+        <v>1600000</v>
+      </c>
+      <c r="K14" s="30" t="s">
+        <v>56</v>
       </c>
       <c r="L14" s="10">
         <v>2860000</v>
@@ -2884,8 +2927,8 @@
       <c r="I15" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="3" t="s">
-        <v>35</v>
+      <c r="J15" s="52">
+        <v>3400000</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
rxns up to cam_ca4 binding to camkii and phospho
</commit_message>
<xml_diff>
--- a/rxns_table.xlsx
+++ b/rxns_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD_2023\CaMKII_hexa_bgnl_to_mcell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A618A38-8E02-40BE-856D-6A386AE4F1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85619136-64D9-4EE1-9C53-2A04689AEF0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4B4FB280-5B08-406D-B059-D87F72317E26}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4B4FB280-5B08-406D-B059-D87F72317E26}"/>
   </bookViews>
   <sheets>
     <sheet name="rxns_table" sheetId="1" r:id="rId1"/>
@@ -38,6 +38,7 @@
     <author>tc={67578144-E3EC-4152-8729-1B44EEC1002D}</author>
     <author>tc={6F7C1780-1EE0-4B0C-B03B-9322192D7EC2}</author>
     <author>tc={802EEB37-19A7-4071-9209-8ED3C607D4E8}</author>
+    <author>tc={CDBBDAF0-DC8A-4716-92BA-AC44BC912388}</author>
     <author>tc={B6F8C469-337C-40BE-B2DC-A13B6B68197A}</author>
     <author>Susana Roman</author>
     <author>tc={6C2818CD-9DCB-407F-A713-A0F009955982}</author>
@@ -72,7 +73,15 @@
 </t>
       </text>
     </comment>
-    <comment ref="B18" authorId="3" shapeId="0" xr:uid="{B6F8C469-337C-40BE-B2DC-A13B6B68197A}">
+    <comment ref="E15" authorId="3" shapeId="0" xr:uid="{CDBBDAF0-DC8A-4716-92BA-AC44BC912388}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Divide it by 2e10-3</t>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="4" shapeId="0" xr:uid="{B6F8C469-337C-40BE-B2DC-A13B6B68197A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -80,7 +89,7 @@
     Not modelled currently; we specify different off rates depending on whether camkii is P or not.</t>
       </text>
     </comment>
-    <comment ref="P19" authorId="4" shapeId="0" xr:uid="{7C16AAE1-EC76-4DE7-BC28-A2AA54E7931D}">
+    <comment ref="P19" authorId="5" shapeId="0" xr:uid="{7C16AAE1-EC76-4DE7-BC28-A2AA54E7931D}">
       <text>
         <r>
           <rPr>
@@ -104,7 +113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N22" authorId="4" shapeId="0" xr:uid="{D783E934-AE8E-45F6-BF32-CFA5F3DEAB20}">
+    <comment ref="N22" authorId="5" shapeId="0" xr:uid="{D783E934-AE8E-45F6-BF32-CFA5F3DEAB20}">
       <text>
         <r>
           <rPr>
@@ -128,7 +137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P25" authorId="5" shapeId="0" xr:uid="{6C2818CD-9DCB-407F-A713-A0F009955982}">
+    <comment ref="P25" authorId="6" shapeId="0" xr:uid="{6C2818CD-9DCB-407F-A713-A0F009955982}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -155,12 +164,6 @@
     <t>CaMKII subunits active/inactive flicker</t>
   </si>
   <si>
-    <t>kon_CaMKII_act</t>
-  </si>
-  <si>
-    <t>koff_CaMKII_inact</t>
-  </si>
-  <si>
     <t>kon_CaM_Ca4_CaMKII</t>
   </si>
   <si>
@@ -312,13 +315,19 @@
   </si>
   <si>
     <t>Rellos et al., 2010</t>
+  </si>
+  <si>
+    <t>kon_CaMKII_open</t>
+  </si>
+  <si>
+    <t>koff_CaMKII_close</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -505,6 +514,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="41">
@@ -1364,6 +1379,9 @@
     <text xml:space="preserve">Range 1.6 and 3.4×106 Mol−1
 </text>
   </threadedComment>
+  <threadedComment ref="E15" dT="2024-09-13T10:39:12.15" personId="{48458BD6-4CAC-498F-B01C-BB6F89FD41FA}" id="{CDBBDAF0-DC8A-4716-92BA-AC44BC912388}">
+    <text>Divide it by 2e10-3</text>
+  </threadedComment>
   <threadedComment ref="B18" dT="2024-08-07T13:14:12.40" personId="{48458BD6-4CAC-498F-B01C-BB6F89FD41FA}" id="{B6F8C469-337C-40BE-B2DC-A13B6B68197A}">
     <text>Not modelled currently; we specify different off rates depending on whether camkii is P or not.</text>
   </threadedComment>
@@ -1378,7 +1396,7 @@
   <dimension ref="A1:CW27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1406,49 +1424,49 @@
         <v>0</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D1" s="36" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="36" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F1" s="36" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H1" s="36" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I1" s="36" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="36" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K1" s="36" t="s">
         <v>2</v>
       </c>
       <c r="L1" s="36" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="M1" s="36" t="s">
         <v>2</v>
       </c>
       <c r="N1" s="36" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="O1" s="36" t="s">
         <v>2</v>
       </c>
       <c r="P1" s="36" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Q1" s="36" t="s">
         <v>2</v>
@@ -1456,22 +1474,22 @@
     </row>
     <row r="2" spans="1:101" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" s="17">
         <v>1000000</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E2" s="17">
         <v>257000000</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G2" s="29">
         <v>25000000</v>
@@ -1480,31 +1498,31 @@
         <v>260000000</v>
       </c>
       <c r="I2" s="30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J2" s="17">
         <v>770000000</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L2" s="24">
         <v>32200000000</v>
       </c>
       <c r="M2" s="25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N2" s="33">
         <v>100000000</v>
       </c>
       <c r="O2" s="34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P2" s="24">
         <v>100000000</v>
       </c>
       <c r="Q2" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R2"/>
       <c r="S2"/>
@@ -1594,19 +1612,19 @@
     <row r="3" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" s="17">
         <v>1000000</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E3" s="17">
         <v>229000</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G3" s="29">
         <v>50000000</v>
@@ -1615,31 +1633,31 @@
         <v>300000000</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J3" s="17">
         <v>32000000000</v>
       </c>
       <c r="K3" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L3" s="24">
         <v>32200000000</v>
       </c>
       <c r="M3" s="25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N3" s="33">
         <v>150000000</v>
       </c>
       <c r="O3" s="34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P3" s="24">
         <v>150000000</v>
       </c>
       <c r="Q3" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R3"/>
       <c r="S3"/>
@@ -1729,19 +1747,19 @@
     <row r="4" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" s="17">
         <v>1000000</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E4" s="17">
         <v>21400000</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G4" s="29">
         <v>1200000</v>
@@ -1750,31 +1768,31 @@
         <v>9600000</v>
       </c>
       <c r="I4" s="30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J4" s="17">
         <v>84000000</v>
       </c>
       <c r="K4" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L4" s="24">
         <v>322000000</v>
       </c>
       <c r="M4" s="25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N4" s="33">
         <v>4000000</v>
       </c>
       <c r="O4" s="34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P4" s="24">
         <v>4000000</v>
       </c>
       <c r="Q4" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R4"/>
       <c r="S4"/>
@@ -1864,19 +1882,19 @@
     <row r="5" spans="1:101" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" s="17">
         <v>1000000</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E5" s="17">
         <v>110000000</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G5" s="29">
         <v>5000000</v>
@@ -1885,31 +1903,31 @@
         <v>25000000</v>
       </c>
       <c r="I5" s="30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J5" s="17">
         <v>250000000</v>
       </c>
       <c r="K5" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L5" s="24">
         <v>322000000</v>
       </c>
       <c r="M5" s="25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N5" s="33">
         <v>10000000</v>
       </c>
       <c r="O5" s="34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P5" s="24">
         <v>10000000</v>
       </c>
       <c r="Q5" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R5"/>
       <c r="S5"/>
@@ -1998,50 +2016,50 @@
     </row>
     <row r="6" spans="1:101" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D6" s="36" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F6" s="36"/>
       <c r="G6" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H6" s="36" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I6" s="36" t="s">
         <v>2</v>
       </c>
       <c r="J6" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K6" s="36" t="s">
         <v>2</v>
       </c>
       <c r="L6" s="36" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M6" s="36" t="s">
         <v>2</v>
       </c>
       <c r="N6" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O6" s="36" t="s">
         <v>2</v>
       </c>
       <c r="P6" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Q6" s="36" t="s">
         <v>2</v>
@@ -2134,19 +2152,19 @@
     <row r="7" spans="1:101" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" s="19">
         <v>1.9279999999999999</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E7" s="17">
         <v>2040</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G7" s="29">
         <v>1000</v>
@@ -2155,31 +2173,31 @@
         <v>4000</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J7" s="17">
         <v>160000</v>
       </c>
       <c r="K7" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L7" s="26">
         <v>9.3800000000000003E-5</v>
       </c>
       <c r="M7" s="25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N7" s="33">
         <v>2660</v>
       </c>
       <c r="O7" s="34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P7" s="24">
         <v>2660</v>
       </c>
       <c r="Q7" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R7"/>
       <c r="S7"/>
@@ -2269,19 +2287,19 @@
     <row r="8" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" s="19">
         <v>1.9370000000000001</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E8" s="17">
         <v>0.39</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G8" s="29">
         <v>500</v>
@@ -2290,31 +2308,31 @@
         <v>1000</v>
       </c>
       <c r="I8" s="30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J8" s="17">
         <v>22000</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L8" s="26">
         <v>9.3800000000000003E-5</v>
       </c>
       <c r="M8" s="25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N8" s="33">
         <v>990</v>
       </c>
       <c r="O8" s="34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P8" s="24">
         <v>990</v>
       </c>
       <c r="Q8" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R8"/>
       <c r="S8"/>
@@ -2404,19 +2422,19 @@
     <row r="9" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" s="19">
         <v>7.476</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E9" s="17">
         <v>742</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G9" s="31">
         <v>10</v>
@@ -2425,31 +2443,31 @@
         <v>70</v>
       </c>
       <c r="I9" s="30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J9" s="17">
         <v>2600</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L9" s="26">
         <v>9.3800000000000003E-5</v>
       </c>
       <c r="M9" s="25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N9" s="35">
         <v>40.24</v>
       </c>
       <c r="O9" s="34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P9" s="28">
         <v>40.24</v>
       </c>
       <c r="Q9" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R9"/>
       <c r="S9"/>
@@ -2539,19 +2557,19 @@
     <row r="10" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" s="19">
         <v>25.783000000000001</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E10" s="17">
         <v>980</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G10" s="31">
         <v>8.5</v>
@@ -2560,31 +2578,31 @@
         <v>10</v>
       </c>
       <c r="I10" s="30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J10" s="19">
         <v>6.5</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L10" s="26">
         <v>9.3800000000000003E-5</v>
       </c>
       <c r="M10" s="25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N10" s="35">
         <v>9.3000000000000007</v>
       </c>
       <c r="O10" s="34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P10" s="28">
         <v>9.3000000000000007</v>
       </c>
       <c r="Q10" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R10"/>
       <c r="S10"/>
@@ -2676,13 +2694,13 @@
         <v>3</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="C11" s="1">
         <v>20000</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
@@ -2696,13 +2714,13 @@
     <row r="12" spans="1:101" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="7" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="C12" s="1">
         <v>10000000</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
@@ -2716,49 +2734,49 @@
     <row r="13" spans="1:101" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="36" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D13" s="36" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="36" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F13" s="36" t="s">
         <v>2</v>
       </c>
       <c r="G13" s="36" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H13" s="36" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I13" s="36" t="s">
         <v>2</v>
       </c>
       <c r="J13" s="36" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K13" s="36" t="s">
         <v>2</v>
       </c>
       <c r="L13" s="36" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="M13" s="36" t="s">
         <v>2</v>
       </c>
       <c r="N13" s="36" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="O13" s="36" t="s">
         <v>2</v>
       </c>
       <c r="P13" s="36" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Q13" s="36" t="s">
         <v>2</v>
@@ -2766,22 +2784,22 @@
     </row>
     <row r="14" spans="1:101" s="2" customFormat="1" ht="33.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C14" s="21">
         <v>4200000</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E14" s="45" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F14" s="45" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G14" s="29">
         <v>1400000</v>
@@ -2790,31 +2808,31 @@
         <v>60000000</v>
       </c>
       <c r="I14" s="30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J14" s="51">
         <v>1600000</v>
       </c>
       <c r="K14" s="30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L14" s="10">
         <v>2860000</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N14" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O14" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P14" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="Q14" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="R14"/>
       <c r="S14"/>
@@ -2904,52 +2922,52 @@
     <row r="15" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D15" s="45" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E15" s="48">
         <v>150000000</v>
       </c>
       <c r="F15" s="49" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H15" s="29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I15" s="30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J15" s="52">
         <v>3400000</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N15" s="33">
         <v>30000000</v>
       </c>
       <c r="O15" s="34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P15" s="24">
         <v>30000000</v>
       </c>
       <c r="Q15" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R15"/>
       <c r="S15" s="15"/>
@@ -3039,52 +3057,52 @@
     <row r="16" spans="1:101" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12"/>
       <c r="B16" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D16" s="45" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E16" s="48">
         <v>50000000</v>
       </c>
       <c r="F16" s="49" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H16" s="29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I16" s="30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N16" s="33">
         <v>10000000</v>
       </c>
       <c r="O16" s="34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P16" s="24">
         <v>50000000</v>
       </c>
       <c r="Q16" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R16"/>
       <c r="S16" s="15"/>
@@ -3177,46 +3195,46 @@
         <v>1</v>
       </c>
       <c r="C17" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D17" s="36" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F17" s="36" t="s">
         <v>2</v>
       </c>
       <c r="G17" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H17" s="36" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I17" s="36" t="s">
         <v>2</v>
       </c>
       <c r="J17" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K17" s="36" t="s">
         <v>2</v>
       </c>
       <c r="L17" s="36" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M17" s="36" t="s">
         <v>2</v>
       </c>
       <c r="N17" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O17" s="36" t="s">
         <v>2</v>
       </c>
       <c r="P17" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Q17" s="36" t="s">
         <v>2</v>
@@ -3308,22 +3326,22 @@
     </row>
     <row r="18" spans="1:101" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C18" s="17">
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E18" s="45" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F18" s="45" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G18" s="31">
         <v>1.1000000000000001</v>
@@ -3332,142 +3350,142 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="I18" s="30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L18" s="9">
         <v>1.1000000000000001</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N18" s="35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O18" s="35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P18" s="28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="Q18" s="27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D19" s="47" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E19" s="50">
         <v>0.46</v>
       </c>
       <c r="F19" s="49" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G19" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H19" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I19" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N19" s="35">
         <v>1.95</v>
       </c>
       <c r="O19" s="34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P19" s="28">
         <v>1.95</v>
       </c>
       <c r="Q19" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:101" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
       <c r="B20" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D20" s="47" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E20" s="48">
         <v>1000</v>
       </c>
       <c r="F20" s="49" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G20" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H20" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I20" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L20" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M20" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N20" s="35">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="O20" s="34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P20" s="24">
         <v>9.0000000000000006E-5</v>
       </c>
       <c r="Q20" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:101" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11"/>
       <c r="B21" s="36" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D21" s="36" t="s">
         <v>2</v>
@@ -3475,34 +3493,34 @@
       <c r="E21" s="36"/>
       <c r="F21" s="36"/>
       <c r="G21" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H21" s="36" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I21" s="36" t="s">
         <v>2</v>
       </c>
       <c r="J21" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K21" s="36" t="s">
         <v>2</v>
       </c>
       <c r="L21" s="36" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="M21" s="36" t="s">
         <v>2</v>
       </c>
       <c r="N21" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O21" s="36" t="s">
         <v>2</v>
       </c>
       <c r="P21" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Q21" s="36" t="s">
         <v>2</v>
@@ -3510,16 +3528,16 @@
     </row>
     <row r="22" spans="1:101" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C22" s="23">
         <v>10</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
@@ -3530,26 +3548,26 @@
         <v>1.25</v>
       </c>
       <c r="I22" s="30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L22" s="3"/>
       <c r="N22" s="35">
         <v>0.96</v>
       </c>
       <c r="O22" s="34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P22" s="28">
         <v>0.96</v>
       </c>
       <c r="Q22" s="27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R22"/>
       <c r="S22"/>
@@ -3606,16 +3624,16 @@
     </row>
     <row r="23" spans="1:101" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C23" s="39">
         <v>0.02</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
@@ -3626,25 +3644,25 @@
         <v>0.05</v>
       </c>
       <c r="I23" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="J23" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="K23" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="J23" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="K23" s="41" t="s">
-        <v>46</v>
-      </c>
       <c r="N23" s="35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O23" s="35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P23" s="28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="Q23" s="28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:101" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3653,7 +3671,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D24" s="36" t="s">
         <v>2</v>
@@ -3661,34 +3679,34 @@
       <c r="E24" s="36"/>
       <c r="F24" s="36"/>
       <c r="G24" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H24" s="36" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I24" s="36" t="s">
         <v>2</v>
       </c>
       <c r="J24" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K24" s="36" t="s">
         <v>2</v>
       </c>
       <c r="L24" s="36" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M24" s="36" t="s">
         <v>2</v>
       </c>
       <c r="N24" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O24" s="36" t="s">
         <v>2</v>
       </c>
       <c r="P24" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Q24" s="16" t="s">
         <v>2</v>
@@ -3696,16 +3714,16 @@
     </row>
     <row r="25" spans="1:101" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C25" s="37">
         <v>20</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
@@ -3719,7 +3737,7 @@
         <v>0.41</v>
       </c>
       <c r="O25" s="34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P25" s="23">
         <v>11.5</v>
@@ -3780,12 +3798,12 @@
     </row>
     <row r="26" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
different file runs all with prob >1 warning
</commit_message>
<xml_diff>
--- a/rxns_table.xlsx
+++ b/rxns_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD_2023\CaMKII_hexa_bgnl_to_mcell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85619136-64D9-4EE1-9C53-2A04689AEF0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E068374F-E8F8-4842-BF2D-5193962F5EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4B4FB280-5B08-406D-B059-D87F72317E26}"/>
+    <workbookView xWindow="41985" yWindow="1830" windowWidth="4995" windowHeight="4005" xr2:uid="{4B4FB280-5B08-406D-B059-D87F72317E26}"/>
   </bookViews>
   <sheets>
     <sheet name="rxns_table" sheetId="1" r:id="rId1"/>
@@ -39,6 +39,7 @@
     <author>tc={6F7C1780-1EE0-4B0C-B03B-9322192D7EC2}</author>
     <author>tc={802EEB37-19A7-4071-9209-8ED3C607D4E8}</author>
     <author>tc={CDBBDAF0-DC8A-4716-92BA-AC44BC912388}</author>
+    <author>tc={B7AC7EFC-29D1-4EF9-AFAD-10D0F49A5243}</author>
     <author>tc={B6F8C469-337C-40BE-B2DC-A13B6B68197A}</author>
     <author>Susana Roman</author>
     <author>tc={6C2818CD-9DCB-407F-A713-A0F009955982}</author>
@@ -78,10 +79,21 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Divide it by 2e10-3</t>
+    Divide it by 2e10-3
+Reply:
+    7.5e10</t>
       </text>
     </comment>
-    <comment ref="B18" authorId="4" shapeId="0" xr:uid="{B6F8C469-337C-40BE-B2DC-A13B6B68197A}">
+    <comment ref="E16" authorId="4" shapeId="0" xr:uid="{B7AC7EFC-29D1-4EF9-AFAD-10D0F49A5243}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    2.5e10
+</t>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="5" shapeId="0" xr:uid="{B6F8C469-337C-40BE-B2DC-A13B6B68197A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -89,7 +101,7 @@
     Not modelled currently; we specify different off rates depending on whether camkii is P or not.</t>
       </text>
     </comment>
-    <comment ref="P19" authorId="5" shapeId="0" xr:uid="{7C16AAE1-EC76-4DE7-BC28-A2AA54E7931D}">
+    <comment ref="P19" authorId="6" shapeId="0" xr:uid="{7C16AAE1-EC76-4DE7-BC28-A2AA54E7931D}">
       <text>
         <r>
           <rPr>
@@ -113,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N22" authorId="5" shapeId="0" xr:uid="{D783E934-AE8E-45F6-BF32-CFA5F3DEAB20}">
+    <comment ref="N22" authorId="6" shapeId="0" xr:uid="{D783E934-AE8E-45F6-BF32-CFA5F3DEAB20}">
       <text>
         <r>
           <rPr>
@@ -137,7 +149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P25" authorId="6" shapeId="0" xr:uid="{6C2818CD-9DCB-407F-A713-A0F009955982}">
+    <comment ref="P25" authorId="7" shapeId="0" xr:uid="{6C2818CD-9DCB-407F-A713-A0F009955982}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1382,6 +1394,13 @@
   <threadedComment ref="E15" dT="2024-09-13T10:39:12.15" personId="{48458BD6-4CAC-498F-B01C-BB6F89FD41FA}" id="{CDBBDAF0-DC8A-4716-92BA-AC44BC912388}">
     <text>Divide it by 2e10-3</text>
   </threadedComment>
+  <threadedComment ref="E15" dT="2024-09-16T17:07:57.32" personId="{48458BD6-4CAC-498F-B01C-BB6F89FD41FA}" id="{CF7BB08E-957E-4036-9AF4-E4A5579A2D2C}" parentId="{CDBBDAF0-DC8A-4716-92BA-AC44BC912388}">
+    <text>7.5e10</text>
+  </threadedComment>
+  <threadedComment ref="E16" dT="2024-09-16T17:08:29.80" personId="{48458BD6-4CAC-498F-B01C-BB6F89FD41FA}" id="{B7AC7EFC-29D1-4EF9-AFAD-10D0F49A5243}">
+    <text xml:space="preserve">2.5e10
+</text>
+  </threadedComment>
   <threadedComment ref="B18" dT="2024-08-07T13:14:12.40" personId="{48458BD6-4CAC-498F-B01C-BB6F89FD41FA}" id="{B6F8C469-337C-40BE-B2DC-A13B6B68197A}">
     <text>Not modelled currently; we specify different off rates depending on whether camkii is P or not.</text>
   </threadedComment>
@@ -1396,7 +1415,7 @@
   <dimension ref="A1:CW27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
corrected way scripts are run
</commit_message>
<xml_diff>
--- a/rxns_table.xlsx
+++ b/rxns_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD_2023\CaMKII_hexa_bgnl_to_mcell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAFDAEBD-64E5-4587-BA4C-91F0C367950D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1A47FB-9C58-4264-BC56-22AADBB24F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="1260" windowWidth="19420" windowHeight="10420" xr2:uid="{4B4FB280-5B08-406D-B059-D87F72317E26}"/>
   </bookViews>
@@ -160,6 +160,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="A23" authorId="7" shapeId="0" xr:uid="{DEC613F9-D75E-482C-AE2A-7E53191AB28B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Susana Roman:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The reaction rate of pT305/306 is over 100-fold slower than
+pT286 (Bradshaw et al., 2002) file:///C:/Users/susan/Downloads/Function_of_CalciumCalmodulin.pdf</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="P25" authorId="8" shapeId="0" xr:uid="{6C2818CD-9DCB-407F-A713-A0F009955982}">
       <text>
         <t>[Threaded comment]
@@ -173,7 +198,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="58">
   <si>
     <t>Description</t>
   </si>
@@ -184,9 +209,6 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>CaMKII subunits active/inactive flicker</t>
-  </si>
-  <si>
     <t>kon_CaM_Ca4_CaMKII</t>
   </si>
   <si>
@@ -344,13 +366,19 @@
   </si>
   <si>
     <t>koff_CaMKII_close</t>
+  </si>
+  <si>
+    <t>CaMKII subunits open/closed flicker</t>
+  </si>
+  <si>
+    <t>Kd=koff/kon= 5e2 (M)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -537,12 +565,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="41">
@@ -1431,8 +1453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B603CBE9-61C1-43B8-82FF-7D32E551985B}">
   <dimension ref="A1:CW27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,49 +1483,49 @@
         <v>0</v>
       </c>
       <c r="B1" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="36" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>13</v>
       </c>
       <c r="D1" s="36" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F1" s="36" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H1" s="36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I1" s="36" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K1" s="36" t="s">
         <v>2</v>
       </c>
       <c r="L1" s="36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M1" s="36" t="s">
         <v>2</v>
       </c>
       <c r="N1" s="36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O1" s="36" t="s">
         <v>2</v>
       </c>
       <c r="P1" s="36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q1" s="36" t="s">
         <v>2</v>
@@ -1511,22 +1533,22 @@
     </row>
     <row r="2" spans="1:101" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="17">
         <v>1000000</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="17">
         <v>257000000</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G2" s="29">
         <v>25000000</v>
@@ -1535,31 +1557,31 @@
         <v>260000000</v>
       </c>
       <c r="I2" s="30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J2" s="17">
         <v>770000000</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L2" s="24">
         <v>32200000000</v>
       </c>
       <c r="M2" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N2" s="33">
         <v>100000000</v>
       </c>
       <c r="O2" s="34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P2" s="24">
         <v>100000000</v>
       </c>
       <c r="Q2" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R2"/>
       <c r="S2"/>
@@ -1649,19 +1671,19 @@
     <row r="3" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="17">
         <v>1000000</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="17">
         <v>229000</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G3" s="29">
         <v>50000000</v>
@@ -1670,31 +1692,31 @@
         <v>300000000</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J3" s="17">
         <v>32000000000</v>
       </c>
       <c r="K3" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L3" s="24">
         <v>32200000000</v>
       </c>
       <c r="M3" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N3" s="33">
         <v>150000000</v>
       </c>
       <c r="O3" s="34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P3" s="24">
         <v>150000000</v>
       </c>
       <c r="Q3" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R3"/>
       <c r="S3"/>
@@ -1784,19 +1806,19 @@
     <row r="4" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="17">
         <v>1000000</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="17">
         <v>21400000</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G4" s="29">
         <v>1200000</v>
@@ -1805,31 +1827,31 @@
         <v>9600000</v>
       </c>
       <c r="I4" s="30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J4" s="17">
         <v>84000000</v>
       </c>
       <c r="K4" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L4" s="24">
         <v>322000000</v>
       </c>
       <c r="M4" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N4" s="33">
         <v>4000000</v>
       </c>
       <c r="O4" s="34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P4" s="24">
         <v>4000000</v>
       </c>
       <c r="Q4" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R4"/>
       <c r="S4"/>
@@ -1919,19 +1941,19 @@
     <row r="5" spans="1:101" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="17">
         <v>1000000</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="17">
         <v>110000000</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G5" s="29">
         <v>5000000</v>
@@ -1940,31 +1962,31 @@
         <v>25000000</v>
       </c>
       <c r="I5" s="30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J5" s="17">
         <v>250000000</v>
       </c>
       <c r="K5" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L5" s="24">
         <v>322000000</v>
       </c>
       <c r="M5" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N5" s="33">
         <v>10000000</v>
       </c>
       <c r="O5" s="34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P5" s="24">
         <v>10000000</v>
       </c>
       <c r="Q5" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R5"/>
       <c r="S5"/>
@@ -2053,50 +2075,50 @@
     </row>
     <row r="6" spans="1:101" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="36" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6" s="36"/>
       <c r="G6" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H6" s="36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I6" s="36" t="s">
         <v>2</v>
       </c>
       <c r="J6" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K6" s="36" t="s">
         <v>2</v>
       </c>
       <c r="L6" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M6" s="36" t="s">
         <v>2</v>
       </c>
       <c r="N6" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O6" s="36" t="s">
         <v>2</v>
       </c>
       <c r="P6" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q6" s="36" t="s">
         <v>2</v>
@@ -2189,19 +2211,19 @@
     <row r="7" spans="1:101" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="19">
         <v>1.9279999999999999</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" s="17">
         <v>2040</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G7" s="29">
         <v>1000</v>
@@ -2210,31 +2232,31 @@
         <v>4000</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J7" s="17">
         <v>160000</v>
       </c>
       <c r="K7" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L7" s="26">
         <v>9.3800000000000003E-5</v>
       </c>
       <c r="M7" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N7" s="33">
         <v>2660</v>
       </c>
       <c r="O7" s="34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P7" s="24">
         <v>2660</v>
       </c>
       <c r="Q7" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R7"/>
       <c r="S7"/>
@@ -2324,19 +2346,19 @@
     <row r="8" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="19">
         <v>1.9370000000000001</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="17">
         <v>0.39</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G8" s="29">
         <v>500</v>
@@ -2345,31 +2367,31 @@
         <v>1000</v>
       </c>
       <c r="I8" s="30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J8" s="17">
         <v>22000</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L8" s="26">
         <v>9.3800000000000003E-5</v>
       </c>
       <c r="M8" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N8" s="33">
         <v>990</v>
       </c>
       <c r="O8" s="34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P8" s="24">
         <v>990</v>
       </c>
       <c r="Q8" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R8"/>
       <c r="S8"/>
@@ -2459,19 +2481,19 @@
     <row r="9" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="19">
         <v>7.476</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="17">
         <v>742</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G9" s="31">
         <v>10</v>
@@ -2480,31 +2502,31 @@
         <v>70</v>
       </c>
       <c r="I9" s="30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J9" s="17">
         <v>2600</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L9" s="26">
         <v>9.3800000000000003E-5</v>
       </c>
       <c r="M9" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N9" s="35">
         <v>40.24</v>
       </c>
       <c r="O9" s="34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P9" s="28">
         <v>40.24</v>
       </c>
       <c r="Q9" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R9"/>
       <c r="S9"/>
@@ -2594,19 +2616,19 @@
     <row r="10" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="19">
         <v>25.783000000000001</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="17">
         <v>980</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G10" s="31">
         <v>8.5</v>
@@ -2615,31 +2637,31 @@
         <v>10</v>
       </c>
       <c r="I10" s="30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J10" s="19">
         <v>6.5</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L10" s="26">
         <v>9.3800000000000003E-5</v>
       </c>
       <c r="M10" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N10" s="35">
         <v>9.3000000000000007</v>
       </c>
       <c r="O10" s="34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P10" s="28">
         <v>9.3000000000000007</v>
       </c>
       <c r="Q10" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R10"/>
       <c r="S10"/>
@@ -2728,16 +2750,16 @@
     </row>
     <row r="11" spans="1:101" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C11" s="1">
         <v>20000</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
@@ -2749,15 +2771,17 @@
       <c r="Q11" s="5"/>
     </row>
     <row r="12" spans="1:101" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
+      <c r="A12" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="B12" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="1">
         <v>10000000</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
@@ -2771,49 +2795,49 @@
     <row r="13" spans="1:101" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="36" t="s">
         <v>12</v>
-      </c>
-      <c r="C13" s="36" t="s">
-        <v>13</v>
       </c>
       <c r="D13" s="36" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" s="36" t="s">
         <v>2</v>
       </c>
       <c r="G13" s="36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H13" s="36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I13" s="36" t="s">
         <v>2</v>
       </c>
       <c r="J13" s="36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K13" s="36" t="s">
         <v>2</v>
       </c>
       <c r="L13" s="36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M13" s="36" t="s">
         <v>2</v>
       </c>
       <c r="N13" s="36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O13" s="36" t="s">
         <v>2</v>
       </c>
       <c r="P13" s="36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q13" s="36" t="s">
         <v>2</v>
@@ -2821,16 +2845,16 @@
     </row>
     <row r="14" spans="1:101" s="2" customFormat="1" ht="33.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" s="21">
         <v>4200000</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E14" s="48">
         <v>150000000</v>
@@ -2846,31 +2870,31 @@
         <v>60000000</v>
       </c>
       <c r="I14" s="30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J14" s="51">
         <v>1600000</v>
       </c>
       <c r="K14" s="30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L14" s="10">
         <v>2860000</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N14" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O14" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P14" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q14" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R14"/>
       <c r="S14"/>
@@ -2960,52 +2984,52 @@
     <row r="15" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" s="45" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E15" s="48">
         <v>150000000</v>
       </c>
       <c r="F15" s="49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H15" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I15" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J15" s="52">
         <v>3400000</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N15" s="33">
         <v>30000000</v>
       </c>
       <c r="O15" s="34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P15" s="24">
         <v>30000000</v>
       </c>
       <c r="Q15" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R15"/>
       <c r="S15" s="15"/>
@@ -3095,52 +3119,52 @@
     <row r="16" spans="1:101" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12"/>
       <c r="B16" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" s="45" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E16" s="48">
         <v>50000000</v>
       </c>
       <c r="F16" s="49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H16" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I16" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N16" s="33">
         <v>10000000</v>
       </c>
       <c r="O16" s="34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P16" s="24">
         <v>50000000</v>
       </c>
       <c r="Q16" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R16"/>
       <c r="S16" s="15"/>
@@ -3233,46 +3257,46 @@
         <v>1</v>
       </c>
       <c r="C17" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D17" s="36" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F17" s="36" t="s">
         <v>2</v>
       </c>
       <c r="G17" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H17" s="36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I17" s="36" t="s">
         <v>2</v>
       </c>
       <c r="J17" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K17" s="36" t="s">
         <v>2</v>
       </c>
       <c r="L17" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M17" s="36" t="s">
         <v>2</v>
       </c>
       <c r="N17" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O17" s="36" t="s">
         <v>2</v>
       </c>
       <c r="P17" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q17" s="36" t="s">
         <v>2</v>
@@ -3364,22 +3388,22 @@
     </row>
     <row r="18" spans="1:101" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="17">
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E18" s="45">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="F18" s="45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G18" s="31">
         <v>1.1000000000000001</v>
@@ -3388,142 +3412,142 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="I18" s="30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L18" s="9">
         <v>1.1000000000000001</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N18" s="35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O18" s="35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P18" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q18" s="27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" s="47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E19" s="50">
         <v>0.46</v>
       </c>
       <c r="F19" s="49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G19" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H19" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I19" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N19" s="35">
         <v>1.95</v>
       </c>
       <c r="O19" s="34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P19" s="28">
         <v>1.95</v>
       </c>
       <c r="Q19" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:101" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
       <c r="B20" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" s="47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E20" s="48">
         <v>1000</v>
       </c>
       <c r="F20" s="49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G20" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H20" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I20" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L20" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M20" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N20" s="35">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="O20" s="34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P20" s="24">
         <v>9.0000000000000006E-5</v>
       </c>
       <c r="Q20" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:101" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11"/>
       <c r="B21" s="36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21" s="36" t="s">
         <v>2</v>
@@ -3531,34 +3555,34 @@
       <c r="E21" s="36"/>
       <c r="F21" s="36"/>
       <c r="G21" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H21" s="36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I21" s="36" t="s">
         <v>2</v>
       </c>
       <c r="J21" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K21" s="36" t="s">
         <v>2</v>
       </c>
       <c r="L21" s="36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M21" s="36" t="s">
         <v>2</v>
       </c>
       <c r="N21" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O21" s="36" t="s">
         <v>2</v>
       </c>
       <c r="P21" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q21" s="36" t="s">
         <v>2</v>
@@ -3566,16 +3590,16 @@
     </row>
     <row r="22" spans="1:101" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="23">
         <v>10</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
@@ -3586,26 +3610,26 @@
         <v>1.25</v>
       </c>
       <c r="I22" s="30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L22" s="3"/>
       <c r="N22" s="35">
         <v>0.96</v>
       </c>
       <c r="O22" s="34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P22" s="28">
         <v>0.96</v>
       </c>
       <c r="Q22" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R22"/>
       <c r="S22"/>
@@ -3662,16 +3686,16 @@
     </row>
     <row r="23" spans="1:101" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C23" s="39">
         <v>0.02</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
@@ -3682,25 +3706,25 @@
         <v>0.05</v>
       </c>
       <c r="I23" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="J23" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="J23" s="40" t="s">
+      <c r="K23" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="K23" s="41" t="s">
-        <v>44</v>
-      </c>
       <c r="N23" s="35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O23" s="35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P23" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q23" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:101" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3709,7 +3733,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D24" s="36" t="s">
         <v>2</v>
@@ -3717,34 +3741,34 @@
       <c r="E24" s="36"/>
       <c r="F24" s="36"/>
       <c r="G24" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H24" s="36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I24" s="36" t="s">
         <v>2</v>
       </c>
       <c r="J24" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K24" s="36" t="s">
         <v>2</v>
       </c>
       <c r="L24" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M24" s="36" t="s">
         <v>2</v>
       </c>
       <c r="N24" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O24" s="36" t="s">
         <v>2</v>
       </c>
       <c r="P24" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q24" s="16" t="s">
         <v>2</v>
@@ -3752,16 +3776,16 @@
     </row>
     <row r="25" spans="1:101" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="37">
         <v>20</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
@@ -3775,7 +3799,7 @@
         <v>0.41</v>
       </c>
       <c r="O25" s="34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P25" s="23">
         <v>11.5</v>
@@ -3836,12 +3860,12 @@
     </row>
     <row r="26" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
need to run files with camkii_nmdar_free recorded
</commit_message>
<xml_diff>
--- a/rxns_table.xlsx
+++ b/rxns_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD_2023\CaMKII_hexa_bgnl_to_mcell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1A47FB-9C58-4264-BC56-22AADBB24F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69633FE-0D97-41F9-9D1A-C74F03CFF48A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="1260" windowWidth="19420" windowHeight="10420" xr2:uid="{4B4FB280-5B08-406D-B059-D87F72317E26}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4B4FB280-5B08-406D-B059-D87F72317E26}"/>
   </bookViews>
   <sheets>
     <sheet name="rxns_table" sheetId="1" r:id="rId1"/>
@@ -796,7 +796,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -911,6 +911,132 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFC000"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFC000"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFFC000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFC000"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFC000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFFC000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFC000"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFFC000"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFC000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFFC000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFFC000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFFC000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -956,7 +1082,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -1020,6 +1146,20 @@
     <xf numFmtId="0" fontId="21" fillId="40" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="21" fillId="38" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="21" fillId="39" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="22" fillId="39" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="39" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="39" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="13" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="11" xfId="13" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="12" xfId="13" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="13" xfId="13" applyBorder="1"/>
+    <xf numFmtId="11" fontId="21" fillId="36" borderId="14" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="22" fillId="36" borderId="15" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="16" xfId="13" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="17" xfId="13" applyBorder="1"/>
+    <xf numFmtId="11" fontId="21" fillId="36" borderId="18" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="22" fillId="36" borderId="19" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1453,32 +1593,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B603CBE9-61C1-43B8-82FF-7D32E551985B}">
   <dimension ref="A1:CW27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="44.1796875" style="4" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" customWidth="1"/>
+    <col min="4" max="5" width="10.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15.81640625" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1"/>
-    <col min="10" max="11" width="11.7109375" customWidth="1"/>
-    <col min="12" max="13" width="11.7109375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" customWidth="1"/>
-    <col min="15" max="17" width="14.5703125" customWidth="1"/>
-    <col min="18" max="18" width="25.28515625" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" customWidth="1"/>
-    <col min="20" max="20" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.26953125" customWidth="1"/>
+    <col min="10" max="11" width="11.7265625" customWidth="1"/>
+    <col min="12" max="13" width="11.7265625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7265625" customWidth="1"/>
+    <col min="15" max="17" width="14.54296875" customWidth="1"/>
+    <col min="18" max="18" width="25.26953125" customWidth="1"/>
+    <col min="19" max="19" width="13.453125" customWidth="1"/>
+    <col min="20" max="20" width="12.1796875" customWidth="1"/>
     <col min="21" max="21" width="11" customWidth="1"/>
-    <col min="22" max="31" width="12.5703125" customWidth="1"/>
+    <col min="22" max="31" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:101" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1488,16 +1628,16 @@
       <c r="C1" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="58" t="s">
         <v>12</v>
       </c>
       <c r="H1" s="36" t="s">
@@ -1531,23 +1671,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:101" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:101" s="2" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="53">
         <v>1000000</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="61">
         <v>257000000</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="62" t="s">
         <v>48</v>
       </c>
       <c r="G2" s="29">
@@ -1668,21 +1808,21 @@
       <c r="CV2"/>
       <c r="CW2"/>
     </row>
-    <row r="3" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12"/>
       <c r="B3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="53">
         <v>1000000</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="61">
         <v>229000</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="62" t="s">
         <v>49</v>
       </c>
       <c r="G3" s="29">
@@ -1803,21 +1943,21 @@
       <c r="CV3"/>
       <c r="CW3"/>
     </row>
-    <row r="4" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12"/>
       <c r="B4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="53">
         <v>1000000</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="61">
         <v>21400000</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="62" t="s">
         <v>50</v>
       </c>
       <c r="G4" s="29">
@@ -1938,21 +2078,21 @@
       <c r="CV4"/>
       <c r="CW4"/>
     </row>
-    <row r="5" spans="1:101" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:101" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="12"/>
       <c r="B5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="53">
         <v>1000000</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="61">
         <v>110000000</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="62" t="s">
         <v>51</v>
       </c>
       <c r="G5" s="29">
@@ -2073,7 +2213,7 @@
       <c r="CV5"/>
       <c r="CW5"/>
     </row>
-    <row r="6" spans="1:101" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:101" s="2" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="12" t="s">
         <v>36</v>
       </c>
@@ -2083,14 +2223,14 @@
       <c r="C6" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36" t="s">
+      <c r="F6" s="64"/>
+      <c r="G6" s="58" t="s">
         <v>20</v>
       </c>
       <c r="H6" s="36" t="s">
@@ -2208,21 +2348,21 @@
       <c r="CV6"/>
       <c r="CW6"/>
     </row>
-    <row r="7" spans="1:101" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:101" s="2" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12"/>
       <c r="B7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="55">
         <v>1.9279999999999999</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="61">
         <v>2040</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="62" t="s">
         <v>48</v>
       </c>
       <c r="G7" s="29">
@@ -2343,21 +2483,21 @@
       <c r="CV7"/>
       <c r="CW7"/>
     </row>
-    <row r="8" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12"/>
       <c r="B8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="55">
         <v>1.9370000000000001</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="61">
         <v>0.39</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="62" t="s">
         <v>49</v>
       </c>
       <c r="G8" s="29">
@@ -2478,21 +2618,21 @@
       <c r="CV8"/>
       <c r="CW8"/>
     </row>
-    <row r="9" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12"/>
       <c r="B9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="55">
         <v>7.476</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="61">
         <v>742</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="62" t="s">
         <v>50</v>
       </c>
       <c r="G9" s="31">
@@ -2613,21 +2753,21 @@
       <c r="CV9"/>
       <c r="CW9"/>
     </row>
-    <row r="10" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:101" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="12"/>
       <c r="B10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="55">
         <v>25.783000000000001</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="65">
         <v>980</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="66" t="s">
         <v>51</v>
       </c>
       <c r="G10" s="31">
@@ -2748,7 +2888,7 @@
       <c r="CV10"/>
       <c r="CW10"/>
     </row>
-    <row r="11" spans="1:101" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:101" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>56</v>
       </c>
@@ -2770,7 +2910,7 @@
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="1:101" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:101" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="11" t="s">
         <v>57</v>
       </c>
@@ -2792,7 +2932,7 @@
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="1:101" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:101" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="11"/>
       <c r="B13" s="36" t="s">
         <v>11</v>
@@ -2843,7 +2983,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:101" s="2" customFormat="1" ht="33.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:101" s="2" customFormat="1" ht="33.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>39</v>
       </c>
@@ -2981,7 +3121,7 @@
       <c r="CV14"/>
       <c r="CW14"/>
     </row>
-    <row r="15" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:101" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="12"/>
       <c r="B15" s="6" t="s">
         <v>33</v>
@@ -3116,7 +3256,7 @@
       <c r="CV15"/>
       <c r="CW15"/>
     </row>
-    <row r="16" spans="1:101" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:101" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="12"/>
       <c r="B16" s="6" t="s">
         <v>34</v>
@@ -3251,7 +3391,7 @@
       <c r="CV16"/>
       <c r="CW16"/>
     </row>
-    <row r="17" spans="1:101" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:101" s="2" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="12"/>
       <c r="B17" s="36" t="s">
         <v>1</v>
@@ -3386,7 +3526,7 @@
       <c r="CV17"/>
       <c r="CW17"/>
     </row>
-    <row r="18" spans="1:101" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:101" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>38</v>
       </c>
@@ -3439,7 +3579,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A19" s="11"/>
       <c r="B19" s="7" t="s">
         <v>4</v>
@@ -3490,7 +3630,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:101" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:101" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="11"/>
       <c r="B20" s="7" t="s">
         <v>5</v>
@@ -3541,7 +3681,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:101" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:101" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="11"/>
       <c r="B21" s="36" t="s">
         <v>11</v>
@@ -3588,7 +3728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:101" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:101" s="2" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
         <v>6</v>
       </c>
@@ -3684,7 +3824,7 @@
       <c r="BP22"/>
       <c r="BQ22"/>
     </row>
-    <row r="23" spans="1:101" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:101" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="11" t="s">
         <v>7</v>
       </c>
@@ -3727,7 +3867,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:101" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:101" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="11"/>
       <c r="B24" s="36" t="s">
         <v>1</v>
@@ -3774,7 +3914,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:101" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:101" s="2" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
         <v>8</v>
       </c>
@@ -3858,12 +3998,12 @@
       <c r="BP25"/>
       <c r="BQ25"/>
     </row>
-    <row r="26" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:101" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>44</v>
       </c>

</xml_diff>